<commit_message>
cfu per gram calc
</commit_message>
<xml_diff>
--- a/inst/Example/Mouse_Experiment_Example.xlsx
+++ b/inst/Example/Mouse_Experiment_Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtcoll06\Box\Lab Docs\R projects\mouseR\inst\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EAADF46-661F-4435-8719-2B13C9F9CB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E156B40-5ED5-4E4F-8F0E-3119265A0E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3608" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3607" uniqueCount="63">
   <si>
     <t>Mouse Weight</t>
   </si>
@@ -20687,15 +20687,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:R47"/>
+  <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="R2" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D1" s="124" t="s">
         <v>50</v>
       </c>
@@ -20712,9 +20712,8 @@
       <c r="O1" s="125"/>
       <c r="P1" s="125"/>
       <c r="Q1" s="125"/>
-      <c r="R1" s="125"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -20766,11 +20765,8 @@
       <c r="Q2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="R2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="121" t="s">
         <v>20</v>
       </c>
@@ -20822,11 +20818,8 @@
       <c r="Q3" s="103">
         <v>500</v>
       </c>
-      <c r="R3" s="103">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="121" t="s">
         <v>20</v>
       </c>
@@ -20838,66 +20831,62 @@
       </c>
       <c r="D4" s="103">
         <f ca="1">RANDBETWEEN(20,60)+D3</f>
-        <v>541</v>
+        <v>552</v>
       </c>
       <c r="E4" s="119">
-        <f t="shared" ref="E4:R4" ca="1" si="0">RANDBETWEEN(20,60)+E3</f>
-        <v>546</v>
+        <f t="shared" ref="E4:Q4" ca="1" si="0">RANDBETWEEN(20,60)+E3</f>
+        <v>552</v>
       </c>
       <c r="F4" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>534</v>
+        <v>522</v>
       </c>
       <c r="G4" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>538</v>
+        <v>559</v>
       </c>
       <c r="H4" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>522</v>
+        <v>545</v>
       </c>
       <c r="I4" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>534</v>
+        <v>558</v>
       </c>
       <c r="J4" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>531</v>
+        <v>551</v>
       </c>
       <c r="K4" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="L4" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="M4" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>540</v>
+        <v>526</v>
       </c>
       <c r="N4" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>522</v>
+        <v>550</v>
       </c>
       <c r="O4" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="P4" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>520</v>
+        <v>544</v>
       </c>
       <c r="Q4" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>525</v>
-      </c>
-      <c r="R4" s="119">
-        <f t="shared" ca="1" si="0"/>
-        <v>528</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="121" t="s">
         <v>20</v>
       </c>
@@ -20908,67 +20897,63 @@
         <v>53</v>
       </c>
       <c r="D5" s="103">
-        <f t="shared" ref="D5:R5" ca="1" si="1">D4-D3</f>
-        <v>41</v>
+        <f t="shared" ref="D5:Q5" ca="1" si="1">D4-D3</f>
+        <v>52</v>
       </c>
       <c r="E5" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="F5" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="G5" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="H5" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="I5" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="J5" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="K5" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L5" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="M5" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="N5" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="O5" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="P5" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="Q5" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="R5" s="103">
-        <f t="shared" ca="1" si="1"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="121" t="s">
         <v>20</v>
       </c>
@@ -21020,11 +21005,8 @@
       <c r="Q6" s="103">
         <v>500</v>
       </c>
-      <c r="R6" s="103">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="121" t="s">
         <v>20</v>
       </c>
@@ -21036,66 +21018,62 @@
       </c>
       <c r="D7" s="119">
         <f ca="1">RANDBETWEEN(20,60)+D6</f>
-        <v>526</v>
+        <v>549</v>
       </c>
       <c r="E7" s="119">
-        <f t="shared" ref="E7:R7" ca="1" si="2">RANDBETWEEN(20,60)+E6</f>
-        <v>547</v>
+        <f t="shared" ref="E7:Q7" ca="1" si="2">RANDBETWEEN(20,60)+E6</f>
+        <v>542</v>
       </c>
       <c r="F7" s="119">
         <f t="shared" ca="1" si="2"/>
-        <v>548</v>
+        <v>536</v>
       </c>
       <c r="G7" s="119">
         <f t="shared" ca="1" si="2"/>
-        <v>548</v>
+        <v>554</v>
       </c>
       <c r="H7" s="119">
         <f t="shared" ca="1" si="2"/>
-        <v>524</v>
+        <v>554</v>
       </c>
       <c r="I7" s="119">
         <f t="shared" ca="1" si="2"/>
-        <v>542</v>
+        <v>552</v>
       </c>
       <c r="J7" s="119">
         <f t="shared" ca="1" si="2"/>
-        <v>532</v>
+        <v>547</v>
       </c>
       <c r="K7" s="119">
         <f t="shared" ca="1" si="2"/>
-        <v>528</v>
+        <v>536</v>
       </c>
       <c r="L7" s="119">
         <f t="shared" ca="1" si="2"/>
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="M7" s="119">
         <f t="shared" ca="1" si="2"/>
-        <v>553</v>
+        <v>520</v>
       </c>
       <c r="N7" s="119">
         <f t="shared" ca="1" si="2"/>
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="O7" s="119">
         <f t="shared" ca="1" si="2"/>
-        <v>527</v>
+        <v>540</v>
       </c>
       <c r="P7" s="119">
         <f t="shared" ca="1" si="2"/>
-        <v>539</v>
+        <v>553</v>
       </c>
       <c r="Q7" s="119">
         <f t="shared" ca="1" si="2"/>
-        <v>530</v>
-      </c>
-      <c r="R7" s="119">
-        <f t="shared" ca="1" si="2"/>
-        <v>546</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="121" t="s">
         <v>20</v>
       </c>
@@ -21106,67 +21084,63 @@
         <v>53</v>
       </c>
       <c r="D8" s="103">
-        <f t="shared" ref="D8:R8" ca="1" si="3">D7-D6</f>
-        <v>26</v>
+        <f t="shared" ref="D8:Q8" ca="1" si="3">D7-D6</f>
+        <v>49</v>
       </c>
       <c r="E8" s="103">
         <f t="shared" ca="1" si="3"/>
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F8" s="103">
         <f t="shared" ca="1" si="3"/>
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="G8" s="103">
         <f t="shared" ca="1" si="3"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="H8" s="103">
         <f t="shared" ca="1" si="3"/>
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="I8" s="103">
         <f t="shared" ca="1" si="3"/>
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="J8" s="103">
         <f t="shared" ca="1" si="3"/>
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="K8" s="103">
         <f t="shared" ca="1" si="3"/>
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="L8" s="103">
         <f t="shared" ca="1" si="3"/>
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M8" s="103">
         <f t="shared" ca="1" si="3"/>
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="N8" s="103">
         <f t="shared" ca="1" si="3"/>
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="O8" s="103">
         <f t="shared" ca="1" si="3"/>
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="P8" s="103">
         <f t="shared" ca="1" si="3"/>
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="Q8" s="103">
         <f t="shared" ca="1" si="3"/>
-        <v>30</v>
-      </c>
-      <c r="R8" s="103">
-        <f t="shared" ca="1" si="3"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="121" t="s">
         <v>20</v>
       </c>
@@ -21218,11 +21192,8 @@
       <c r="Q9" s="103">
         <v>500</v>
       </c>
-      <c r="R9" s="103">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="121" t="s">
         <v>20</v>
       </c>
@@ -21234,66 +21205,62 @@
       </c>
       <c r="D10" s="103">
         <f ca="1">RANDBETWEEN(20,60)+D9</f>
-        <v>527</v>
+        <v>550</v>
       </c>
       <c r="E10" s="119">
-        <f t="shared" ref="E10:R10" ca="1" si="4">RANDBETWEEN(20,60)+E9</f>
-        <v>528</v>
+        <f t="shared" ref="E10:Q10" ca="1" si="4">RANDBETWEEN(20,60)+E9</f>
+        <v>546</v>
       </c>
       <c r="F10" s="119">
         <f t="shared" ca="1" si="4"/>
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="G10" s="119">
         <f t="shared" ca="1" si="4"/>
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="H10" s="119">
         <f t="shared" ca="1" si="4"/>
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="I10" s="119">
         <f t="shared" ca="1" si="4"/>
-        <v>523</v>
+        <v>531</v>
       </c>
       <c r="J10" s="119">
         <f t="shared" ca="1" si="4"/>
-        <v>530</v>
+        <v>540</v>
       </c>
       <c r="K10" s="119">
         <f t="shared" ca="1" si="4"/>
-        <v>543</v>
+        <v>533</v>
       </c>
       <c r="L10" s="119">
         <f t="shared" ca="1" si="4"/>
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="M10" s="119">
         <f t="shared" ca="1" si="4"/>
-        <v>531</v>
+        <v>542</v>
       </c>
       <c r="N10" s="119">
         <f t="shared" ca="1" si="4"/>
-        <v>526</v>
+        <v>546</v>
       </c>
       <c r="O10" s="119">
         <f t="shared" ca="1" si="4"/>
-        <v>520</v>
+        <v>556</v>
       </c>
       <c r="P10" s="119">
         <f t="shared" ca="1" si="4"/>
-        <v>559</v>
+        <v>520</v>
       </c>
       <c r="Q10" s="119">
         <f t="shared" ca="1" si="4"/>
-        <v>529</v>
-      </c>
-      <c r="R10" s="119">
-        <f t="shared" ca="1" si="4"/>
-        <v>531</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="121" t="s">
         <v>20</v>
       </c>
@@ -21304,67 +21271,63 @@
         <v>53</v>
       </c>
       <c r="D11" s="103">
-        <f t="shared" ref="D11:R11" ca="1" si="5">D10-D9</f>
-        <v>27</v>
+        <f t="shared" ref="D11:Q11" ca="1" si="5">D10-D9</f>
+        <v>50</v>
       </c>
       <c r="E11" s="103">
         <f t="shared" ca="1" si="5"/>
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="F11" s="103">
         <f t="shared" ca="1" si="5"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G11" s="103">
         <f t="shared" ca="1" si="5"/>
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="H11" s="103">
         <f t="shared" ca="1" si="5"/>
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="I11" s="103">
         <f t="shared" ca="1" si="5"/>
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="J11" s="103">
         <f t="shared" ca="1" si="5"/>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="K11" s="103">
         <f t="shared" ca="1" si="5"/>
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="L11" s="103">
         <f t="shared" ca="1" si="5"/>
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="M11" s="103">
         <f t="shared" ca="1" si="5"/>
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="N11" s="103">
         <f t="shared" ca="1" si="5"/>
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="O11" s="103">
         <f t="shared" ca="1" si="5"/>
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="P11" s="103">
         <f t="shared" ca="1" si="5"/>
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="Q11" s="103">
         <f t="shared" ca="1" si="5"/>
-        <v>29</v>
-      </c>
-      <c r="R11" s="103">
-        <f t="shared" ca="1" si="5"/>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="121" t="s">
         <v>20</v>
       </c>
@@ -21416,11 +21379,8 @@
       <c r="Q12" s="103">
         <v>500</v>
       </c>
-      <c r="R12" s="103">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="121" t="s">
         <v>20</v>
       </c>
@@ -21432,66 +21392,62 @@
       </c>
       <c r="D13" s="119">
         <f ca="1">RANDBETWEEN(20,60)+D12</f>
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="E13" s="119">
         <f t="shared" ref="E13" ca="1" si="6">RANDBETWEEN(20,60)+E12</f>
-        <v>528</v>
+        <v>558</v>
       </c>
       <c r="F13" s="119">
         <f t="shared" ref="F13" ca="1" si="7">RANDBETWEEN(20,60)+F12</f>
-        <v>555</v>
+        <v>546</v>
       </c>
       <c r="G13" s="119">
         <f t="shared" ref="G13" ca="1" si="8">RANDBETWEEN(20,60)+G12</f>
-        <v>533</v>
+        <v>546</v>
       </c>
       <c r="H13" s="119">
         <f t="shared" ref="H13" ca="1" si="9">RANDBETWEEN(20,60)+H12</f>
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="I13" s="119">
         <f t="shared" ref="I13" ca="1" si="10">RANDBETWEEN(20,60)+I12</f>
-        <v>556</v>
+        <v>525</v>
       </c>
       <c r="J13" s="119">
         <f t="shared" ref="J13" ca="1" si="11">RANDBETWEEN(20,60)+J12</f>
-        <v>535</v>
+        <v>525</v>
       </c>
       <c r="K13" s="119">
         <f t="shared" ref="K13" ca="1" si="12">RANDBETWEEN(20,60)+K12</f>
-        <v>523</v>
+        <v>547</v>
       </c>
       <c r="L13" s="119">
         <f t="shared" ref="L13" ca="1" si="13">RANDBETWEEN(20,60)+L12</f>
-        <v>532</v>
+        <v>547</v>
       </c>
       <c r="M13" s="119">
         <f t="shared" ref="M13" ca="1" si="14">RANDBETWEEN(20,60)+M12</f>
-        <v>532</v>
+        <v>537</v>
       </c>
       <c r="N13" s="119">
         <f t="shared" ref="N13" ca="1" si="15">RANDBETWEEN(20,60)+N12</f>
-        <v>525</v>
+        <v>546</v>
       </c>
       <c r="O13" s="119">
         <f t="shared" ref="O13" ca="1" si="16">RANDBETWEEN(20,60)+O12</f>
-        <v>531</v>
+        <v>537</v>
       </c>
       <c r="P13" s="119">
         <f t="shared" ref="P13" ca="1" si="17">RANDBETWEEN(20,60)+P12</f>
-        <v>553</v>
+        <v>538</v>
       </c>
       <c r="Q13" s="119">
         <f t="shared" ref="Q13" ca="1" si="18">RANDBETWEEN(20,60)+Q12</f>
-        <v>559</v>
-      </c>
-      <c r="R13" s="119">
-        <f t="shared" ref="R13" ca="1" si="19">RANDBETWEEN(20,60)+R12</f>
-        <v>541</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="121" t="s">
         <v>20</v>
       </c>
@@ -21502,67 +21458,63 @@
         <v>53</v>
       </c>
       <c r="D14" s="103">
-        <f t="shared" ref="D14:R14" ca="1" si="20">D13-D12</f>
-        <v>54</v>
+        <f t="shared" ref="D14:Q14" ca="1" si="19">D13-D12</f>
+        <v>50</v>
       </c>
       <c r="E14" s="103">
-        <f t="shared" ca="1" si="20"/>
-        <v>28</v>
+        <f t="shared" ca="1" si="19"/>
+        <v>58</v>
       </c>
       <c r="F14" s="103">
-        <f t="shared" ca="1" si="20"/>
-        <v>55</v>
+        <f t="shared" ca="1" si="19"/>
+        <v>46</v>
       </c>
       <c r="G14" s="103">
-        <f t="shared" ca="1" si="20"/>
-        <v>33</v>
+        <f t="shared" ca="1" si="19"/>
+        <v>46</v>
       </c>
       <c r="H14" s="103">
-        <f t="shared" ca="1" si="20"/>
-        <v>52</v>
+        <f t="shared" ca="1" si="19"/>
+        <v>49</v>
       </c>
       <c r="I14" s="103">
-        <f t="shared" ca="1" si="20"/>
-        <v>56</v>
+        <f t="shared" ca="1" si="19"/>
+        <v>25</v>
       </c>
       <c r="J14" s="103">
-        <f t="shared" ca="1" si="20"/>
-        <v>35</v>
+        <f t="shared" ca="1" si="19"/>
+        <v>25</v>
       </c>
       <c r="K14" s="103">
-        <f t="shared" ca="1" si="20"/>
-        <v>23</v>
+        <f t="shared" ca="1" si="19"/>
+        <v>47</v>
       </c>
       <c r="L14" s="103">
-        <f t="shared" ca="1" si="20"/>
-        <v>32</v>
+        <f t="shared" ca="1" si="19"/>
+        <v>47</v>
       </c>
       <c r="M14" s="103">
-        <f t="shared" ca="1" si="20"/>
-        <v>32</v>
+        <f t="shared" ca="1" si="19"/>
+        <v>37</v>
       </c>
       <c r="N14" s="103">
-        <f t="shared" ca="1" si="20"/>
-        <v>25</v>
+        <f t="shared" ca="1" si="19"/>
+        <v>46</v>
       </c>
       <c r="O14" s="103">
-        <f t="shared" ca="1" si="20"/>
-        <v>31</v>
+        <f t="shared" ca="1" si="19"/>
+        <v>37</v>
       </c>
       <c r="P14" s="103">
-        <f t="shared" ca="1" si="20"/>
-        <v>53</v>
+        <f t="shared" ca="1" si="19"/>
+        <v>38</v>
       </c>
       <c r="Q14" s="103">
-        <f t="shared" ca="1" si="20"/>
-        <v>59</v>
-      </c>
-      <c r="R14" s="103">
-        <f t="shared" ca="1" si="20"/>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="19"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="121" t="s">
         <v>20</v>
       </c>
@@ -21614,11 +21566,8 @@
       <c r="Q15" s="103">
         <v>500</v>
       </c>
-      <c r="R15" s="103">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="121" t="s">
         <v>20</v>
       </c>
@@ -21630,66 +21579,62 @@
       </c>
       <c r="D16" s="119">
         <f ca="1">RANDBETWEEN(20,60)+D15</f>
-        <v>531</v>
+        <v>558</v>
       </c>
       <c r="E16" s="119">
-        <f t="shared" ref="E16" ca="1" si="21">RANDBETWEEN(20,60)+E15</f>
-        <v>527</v>
+        <f t="shared" ref="E16" ca="1" si="20">RANDBETWEEN(20,60)+E15</f>
+        <v>548</v>
       </c>
       <c r="F16" s="119">
-        <f t="shared" ref="F16" ca="1" si="22">RANDBETWEEN(20,60)+F15</f>
-        <v>530</v>
+        <f t="shared" ref="F16" ca="1" si="21">RANDBETWEEN(20,60)+F15</f>
+        <v>524</v>
       </c>
       <c r="G16" s="119">
-        <f t="shared" ref="G16" ca="1" si="23">RANDBETWEEN(20,60)+G15</f>
-        <v>532</v>
+        <f t="shared" ref="G16" ca="1" si="22">RANDBETWEEN(20,60)+G15</f>
+        <v>541</v>
       </c>
       <c r="H16" s="119">
-        <f t="shared" ref="H16" ca="1" si="24">RANDBETWEEN(20,60)+H15</f>
-        <v>538</v>
+        <f t="shared" ref="H16" ca="1" si="23">RANDBETWEEN(20,60)+H15</f>
+        <v>537</v>
       </c>
       <c r="I16" s="119">
-        <f t="shared" ref="I16" ca="1" si="25">RANDBETWEEN(20,60)+I15</f>
+        <f t="shared" ref="I16" ca="1" si="24">RANDBETWEEN(20,60)+I15</f>
+        <v>521</v>
+      </c>
+      <c r="J16" s="119">
+        <f t="shared" ref="J16" ca="1" si="25">RANDBETWEEN(20,60)+J15</f>
+        <v>558</v>
+      </c>
+      <c r="K16" s="119">
+        <f t="shared" ref="K16" ca="1" si="26">RANDBETWEEN(20,60)+K15</f>
+        <v>533</v>
+      </c>
+      <c r="L16" s="119">
+        <f t="shared" ref="L16" ca="1" si="27">RANDBETWEEN(20,60)+L15</f>
+        <v>537</v>
+      </c>
+      <c r="M16" s="119">
+        <f t="shared" ref="M16" ca="1" si="28">RANDBETWEEN(20,60)+M15</f>
+        <v>540</v>
+      </c>
+      <c r="N16" s="119">
+        <f t="shared" ref="N16" ca="1" si="29">RANDBETWEEN(20,60)+N15</f>
+        <v>555</v>
+      </c>
+      <c r="O16" s="119">
+        <f t="shared" ref="O16" ca="1" si="30">RANDBETWEEN(20,60)+O15</f>
+        <v>549</v>
+      </c>
+      <c r="P16" s="119">
+        <f t="shared" ref="P16" ca="1" si="31">RANDBETWEEN(20,60)+P15</f>
+        <v>554</v>
+      </c>
+      <c r="Q16" s="119">
+        <f t="shared" ref="Q16" ca="1" si="32">RANDBETWEEN(20,60)+Q15</f>
         <v>559</v>
       </c>
-      <c r="J16" s="119">
-        <f t="shared" ref="J16" ca="1" si="26">RANDBETWEEN(20,60)+J15</f>
-        <v>542</v>
-      </c>
-      <c r="K16" s="119">
-        <f t="shared" ref="K16" ca="1" si="27">RANDBETWEEN(20,60)+K15</f>
-        <v>527</v>
-      </c>
-      <c r="L16" s="119">
-        <f t="shared" ref="L16" ca="1" si="28">RANDBETWEEN(20,60)+L15</f>
-        <v>557</v>
-      </c>
-      <c r="M16" s="119">
-        <f t="shared" ref="M16" ca="1" si="29">RANDBETWEEN(20,60)+M15</f>
-        <v>547</v>
-      </c>
-      <c r="N16" s="119">
-        <f t="shared" ref="N16" ca="1" si="30">RANDBETWEEN(20,60)+N15</f>
-        <v>543</v>
-      </c>
-      <c r="O16" s="119">
-        <f t="shared" ref="O16" ca="1" si="31">RANDBETWEEN(20,60)+O15</f>
-        <v>540</v>
-      </c>
-      <c r="P16" s="119">
-        <f t="shared" ref="P16" ca="1" si="32">RANDBETWEEN(20,60)+P15</f>
-        <v>556</v>
-      </c>
-      <c r="Q16" s="119">
-        <f t="shared" ref="Q16" ca="1" si="33">RANDBETWEEN(20,60)+Q15</f>
-        <v>534</v>
-      </c>
-      <c r="R16" s="119">
-        <f t="shared" ref="R16" ca="1" si="34">RANDBETWEEN(20,60)+R15</f>
-        <v>534</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="121" t="s">
         <v>20</v>
       </c>
@@ -21700,67 +21645,63 @@
         <v>53</v>
       </c>
       <c r="D17" s="103">
-        <f t="shared" ref="D17:R17" ca="1" si="35">D16-D15</f>
-        <v>31</v>
+        <f t="shared" ref="D17:Q17" ca="1" si="33">D16-D15</f>
+        <v>58</v>
       </c>
       <c r="E17" s="103">
-        <f t="shared" ca="1" si="35"/>
-        <v>27</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>48</v>
       </c>
       <c r="F17" s="103">
-        <f t="shared" ca="1" si="35"/>
-        <v>30</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>24</v>
       </c>
       <c r="G17" s="103">
-        <f t="shared" ca="1" si="35"/>
-        <v>32</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>41</v>
       </c>
       <c r="H17" s="103">
-        <f t="shared" ca="1" si="35"/>
-        <v>38</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>37</v>
       </c>
       <c r="I17" s="103">
-        <f t="shared" ca="1" si="35"/>
+        <f t="shared" ca="1" si="33"/>
+        <v>21</v>
+      </c>
+      <c r="J17" s="103">
+        <f t="shared" ca="1" si="33"/>
+        <v>58</v>
+      </c>
+      <c r="K17" s="103">
+        <f t="shared" ca="1" si="33"/>
+        <v>33</v>
+      </c>
+      <c r="L17" s="103">
+        <f t="shared" ca="1" si="33"/>
+        <v>37</v>
+      </c>
+      <c r="M17" s="103">
+        <f t="shared" ca="1" si="33"/>
+        <v>40</v>
+      </c>
+      <c r="N17" s="103">
+        <f t="shared" ca="1" si="33"/>
+        <v>55</v>
+      </c>
+      <c r="O17" s="103">
+        <f t="shared" ca="1" si="33"/>
+        <v>49</v>
+      </c>
+      <c r="P17" s="103">
+        <f t="shared" ca="1" si="33"/>
+        <v>54</v>
+      </c>
+      <c r="Q17" s="103">
+        <f t="shared" ca="1" si="33"/>
         <v>59</v>
       </c>
-      <c r="J17" s="103">
-        <f t="shared" ca="1" si="35"/>
-        <v>42</v>
-      </c>
-      <c r="K17" s="103">
-        <f t="shared" ca="1" si="35"/>
-        <v>27</v>
-      </c>
-      <c r="L17" s="103">
-        <f t="shared" ca="1" si="35"/>
-        <v>57</v>
-      </c>
-      <c r="M17" s="103">
-        <f t="shared" ca="1" si="35"/>
-        <v>47</v>
-      </c>
-      <c r="N17" s="103">
-        <f t="shared" ca="1" si="35"/>
-        <v>43</v>
-      </c>
-      <c r="O17" s="103">
-        <f t="shared" ca="1" si="35"/>
-        <v>40</v>
-      </c>
-      <c r="P17" s="103">
-        <f t="shared" ca="1" si="35"/>
-        <v>56</v>
-      </c>
-      <c r="Q17" s="103">
-        <f t="shared" ca="1" si="35"/>
-        <v>34</v>
-      </c>
-      <c r="R17" s="103">
-        <f t="shared" ca="1" si="35"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="122" t="s">
         <v>26</v>
       </c>
@@ -21812,11 +21753,8 @@
       <c r="Q18" s="104">
         <v>500</v>
       </c>
-      <c r="R18" s="104">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="122" t="s">
         <v>26</v>
       </c>
@@ -21828,66 +21766,62 @@
       </c>
       <c r="D19" s="104">
         <f ca="1">RANDBETWEEN(20,60)+D18</f>
-        <v>520</v>
+        <v>542</v>
       </c>
       <c r="E19" s="104">
-        <f t="shared" ref="E19" ca="1" si="36">RANDBETWEEN(20,60)+E18</f>
-        <v>536</v>
+        <f t="shared" ref="E19" ca="1" si="34">RANDBETWEEN(20,60)+E18</f>
+        <v>523</v>
       </c>
       <c r="F19" s="104">
-        <f t="shared" ref="F19" ca="1" si="37">RANDBETWEEN(20,60)+F18</f>
-        <v>520</v>
+        <f t="shared" ref="F19" ca="1" si="35">RANDBETWEEN(20,60)+F18</f>
+        <v>547</v>
       </c>
       <c r="G19" s="104">
-        <f t="shared" ref="G19" ca="1" si="38">RANDBETWEEN(20,60)+G18</f>
-        <v>532</v>
+        <f t="shared" ref="G19" ca="1" si="36">RANDBETWEEN(20,60)+G18</f>
+        <v>544</v>
       </c>
       <c r="H19" s="104">
-        <f t="shared" ref="H19" ca="1" si="39">RANDBETWEEN(20,60)+H18</f>
+        <f t="shared" ref="H19" ca="1" si="37">RANDBETWEEN(20,60)+H18</f>
+        <v>528</v>
+      </c>
+      <c r="I19" s="104">
+        <f t="shared" ref="I19" ca="1" si="38">RANDBETWEEN(20,60)+I18</f>
+        <v>525</v>
+      </c>
+      <c r="J19" s="104">
+        <f t="shared" ref="J19" ca="1" si="39">RANDBETWEEN(20,60)+J18</f>
+        <v>560</v>
+      </c>
+      <c r="K19" s="104">
+        <f t="shared" ref="K19" ca="1" si="40">RANDBETWEEN(20,60)+K18</f>
+        <v>556</v>
+      </c>
+      <c r="L19" s="104">
+        <f t="shared" ref="L19" ca="1" si="41">RANDBETWEEN(20,60)+L18</f>
+        <v>545</v>
+      </c>
+      <c r="M19" s="104">
+        <f t="shared" ref="M19" ca="1" si="42">RANDBETWEEN(20,60)+M18</f>
+        <v>545</v>
+      </c>
+      <c r="N19" s="104">
+        <f t="shared" ref="N19" ca="1" si="43">RANDBETWEEN(20,60)+N18</f>
+        <v>524</v>
+      </c>
+      <c r="O19" s="104">
+        <f t="shared" ref="O19" ca="1" si="44">RANDBETWEEN(20,60)+O18</f>
+        <v>541</v>
+      </c>
+      <c r="P19" s="104">
+        <f t="shared" ref="P19" ca="1" si="45">RANDBETWEEN(20,60)+P18</f>
         <v>531</v>
       </c>
-      <c r="I19" s="104">
-        <f t="shared" ref="I19" ca="1" si="40">RANDBETWEEN(20,60)+I18</f>
-        <v>527</v>
-      </c>
-      <c r="J19" s="104">
-        <f t="shared" ref="J19" ca="1" si="41">RANDBETWEEN(20,60)+J18</f>
-        <v>554</v>
-      </c>
-      <c r="K19" s="104">
-        <f t="shared" ref="K19" ca="1" si="42">RANDBETWEEN(20,60)+K18</f>
-        <v>534</v>
-      </c>
-      <c r="L19" s="104">
-        <f t="shared" ref="L19" ca="1" si="43">RANDBETWEEN(20,60)+L18</f>
-        <v>536</v>
-      </c>
-      <c r="M19" s="104">
-        <f t="shared" ref="M19" ca="1" si="44">RANDBETWEEN(20,60)+M18</f>
-        <v>533</v>
-      </c>
-      <c r="N19" s="104">
-        <f t="shared" ref="N19" ca="1" si="45">RANDBETWEEN(20,60)+N18</f>
-        <v>542</v>
-      </c>
-      <c r="O19" s="104">
-        <f t="shared" ref="O19" ca="1" si="46">RANDBETWEEN(20,60)+O18</f>
-        <v>540</v>
-      </c>
-      <c r="P19" s="104">
-        <f t="shared" ref="P19" ca="1" si="47">RANDBETWEEN(20,60)+P18</f>
-        <v>559</v>
-      </c>
       <c r="Q19" s="104">
-        <f t="shared" ref="Q19" ca="1" si="48">RANDBETWEEN(20,60)+Q18</f>
-        <v>527</v>
-      </c>
-      <c r="R19" s="104">
-        <f t="shared" ref="R19" ca="1" si="49">RANDBETWEEN(20,60)+R18</f>
-        <v>558</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" ref="Q19" ca="1" si="46">RANDBETWEEN(20,60)+Q18</f>
+        <v>548</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="122" t="s">
         <v>26</v>
       </c>
@@ -21898,67 +21832,63 @@
         <v>53</v>
       </c>
       <c r="D20" s="104">
-        <f t="shared" ref="D20:R20" ca="1" si="50">D19-D18</f>
-        <v>20</v>
+        <f t="shared" ref="D20:Q20" ca="1" si="47">D19-D18</f>
+        <v>42</v>
       </c>
       <c r="E20" s="104">
-        <f t="shared" ca="1" si="50"/>
-        <v>36</v>
+        <f t="shared" ca="1" si="47"/>
+        <v>23</v>
       </c>
       <c r="F20" s="104">
-        <f t="shared" ca="1" si="50"/>
-        <v>20</v>
+        <f t="shared" ca="1" si="47"/>
+        <v>47</v>
       </c>
       <c r="G20" s="104">
-        <f t="shared" ca="1" si="50"/>
-        <v>32</v>
+        <f t="shared" ca="1" si="47"/>
+        <v>44</v>
       </c>
       <c r="H20" s="104">
-        <f t="shared" ca="1" si="50"/>
+        <f t="shared" ca="1" si="47"/>
+        <v>28</v>
+      </c>
+      <c r="I20" s="104">
+        <f t="shared" ca="1" si="47"/>
+        <v>25</v>
+      </c>
+      <c r="J20" s="104">
+        <f t="shared" ca="1" si="47"/>
+        <v>60</v>
+      </c>
+      <c r="K20" s="104">
+        <f t="shared" ca="1" si="47"/>
+        <v>56</v>
+      </c>
+      <c r="L20" s="104">
+        <f t="shared" ca="1" si="47"/>
+        <v>45</v>
+      </c>
+      <c r="M20" s="104">
+        <f t="shared" ca="1" si="47"/>
+        <v>45</v>
+      </c>
+      <c r="N20" s="104">
+        <f t="shared" ca="1" si="47"/>
+        <v>24</v>
+      </c>
+      <c r="O20" s="104">
+        <f t="shared" ca="1" si="47"/>
+        <v>41</v>
+      </c>
+      <c r="P20" s="104">
+        <f t="shared" ca="1" si="47"/>
         <v>31</v>
       </c>
-      <c r="I20" s="104">
-        <f t="shared" ca="1" si="50"/>
-        <v>27</v>
-      </c>
-      <c r="J20" s="104">
-        <f t="shared" ca="1" si="50"/>
-        <v>54</v>
-      </c>
-      <c r="K20" s="104">
-        <f t="shared" ca="1" si="50"/>
-        <v>34</v>
-      </c>
-      <c r="L20" s="104">
-        <f t="shared" ca="1" si="50"/>
-        <v>36</v>
-      </c>
-      <c r="M20" s="104">
-        <f t="shared" ca="1" si="50"/>
-        <v>33</v>
-      </c>
-      <c r="N20" s="104">
-        <f t="shared" ca="1" si="50"/>
-        <v>42</v>
-      </c>
-      <c r="O20" s="104">
-        <f t="shared" ca="1" si="50"/>
-        <v>40</v>
-      </c>
-      <c r="P20" s="104">
-        <f t="shared" ca="1" si="50"/>
-        <v>59</v>
-      </c>
       <c r="Q20" s="104">
-        <f t="shared" ca="1" si="50"/>
-        <v>27</v>
-      </c>
-      <c r="R20" s="104">
-        <f t="shared" ca="1" si="50"/>
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="47"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="122" t="s">
         <v>26</v>
       </c>
@@ -22010,11 +21940,8 @@
       <c r="Q21" s="104">
         <v>500</v>
       </c>
-      <c r="R21" s="104">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="122" t="s">
         <v>26</v>
       </c>
@@ -22026,66 +21953,62 @@
       </c>
       <c r="D22" s="104">
         <f ca="1">RANDBETWEEN(20,60)+D21</f>
-        <v>554</v>
+        <v>528</v>
       </c>
       <c r="E22" s="104">
-        <f t="shared" ref="E22" ca="1" si="51">RANDBETWEEN(20,60)+E21</f>
-        <v>544</v>
+        <f t="shared" ref="E22" ca="1" si="48">RANDBETWEEN(20,60)+E21</f>
+        <v>535</v>
       </c>
       <c r="F22" s="104">
-        <f t="shared" ref="F22" ca="1" si="52">RANDBETWEEN(20,60)+F21</f>
-        <v>548</v>
+        <f t="shared" ref="F22" ca="1" si="49">RANDBETWEEN(20,60)+F21</f>
+        <v>532</v>
       </c>
       <c r="G22" s="104">
-        <f t="shared" ref="G22" ca="1" si="53">RANDBETWEEN(20,60)+G21</f>
-        <v>521</v>
+        <f t="shared" ref="G22" ca="1" si="50">RANDBETWEEN(20,60)+G21</f>
+        <v>545</v>
       </c>
       <c r="H22" s="104">
-        <f t="shared" ref="H22" ca="1" si="54">RANDBETWEEN(20,60)+H21</f>
-        <v>541</v>
+        <f t="shared" ref="H22" ca="1" si="51">RANDBETWEEN(20,60)+H21</f>
+        <v>560</v>
       </c>
       <c r="I22" s="104">
-        <f t="shared" ref="I22" ca="1" si="55">RANDBETWEEN(20,60)+I21</f>
-        <v>542</v>
+        <f t="shared" ref="I22" ca="1" si="52">RANDBETWEEN(20,60)+I21</f>
+        <v>520</v>
       </c>
       <c r="J22" s="104">
-        <f t="shared" ref="J22" ca="1" si="56">RANDBETWEEN(20,60)+J21</f>
-        <v>532</v>
+        <f t="shared" ref="J22" ca="1" si="53">RANDBETWEEN(20,60)+J21</f>
+        <v>535</v>
       </c>
       <c r="K22" s="104">
-        <f t="shared" ref="K22" ca="1" si="57">RANDBETWEEN(20,60)+K21</f>
-        <v>542</v>
+        <f t="shared" ref="K22" ca="1" si="54">RANDBETWEEN(20,60)+K21</f>
+        <v>556</v>
       </c>
       <c r="L22" s="104">
-        <f t="shared" ref="L22" ca="1" si="58">RANDBETWEEN(20,60)+L21</f>
-        <v>521</v>
+        <f t="shared" ref="L22" ca="1" si="55">RANDBETWEEN(20,60)+L21</f>
+        <v>539</v>
       </c>
       <c r="M22" s="104">
-        <f t="shared" ref="M22" ca="1" si="59">RANDBETWEEN(20,60)+M21</f>
-        <v>556</v>
+        <f t="shared" ref="M22" ca="1" si="56">RANDBETWEEN(20,60)+M21</f>
+        <v>522</v>
       </c>
       <c r="N22" s="104">
-        <f t="shared" ref="N22" ca="1" si="60">RANDBETWEEN(20,60)+N21</f>
-        <v>532</v>
+        <f t="shared" ref="N22" ca="1" si="57">RANDBETWEEN(20,60)+N21</f>
+        <v>528</v>
       </c>
       <c r="O22" s="104">
-        <f t="shared" ref="O22" ca="1" si="61">RANDBETWEEN(20,60)+O21</f>
-        <v>537</v>
+        <f t="shared" ref="O22" ca="1" si="58">RANDBETWEEN(20,60)+O21</f>
+        <v>523</v>
       </c>
       <c r="P22" s="104">
-        <f t="shared" ref="P22" ca="1" si="62">RANDBETWEEN(20,60)+P21</f>
-        <v>531</v>
+        <f t="shared" ref="P22" ca="1" si="59">RANDBETWEEN(20,60)+P21</f>
+        <v>540</v>
       </c>
       <c r="Q22" s="104">
-        <f t="shared" ref="Q22" ca="1" si="63">RANDBETWEEN(20,60)+Q21</f>
-        <v>524</v>
-      </c>
-      <c r="R22" s="104">
-        <f t="shared" ref="R22" ca="1" si="64">RANDBETWEEN(20,60)+R21</f>
-        <v>527</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" ref="Q22" ca="1" si="60">RANDBETWEEN(20,60)+Q21</f>
+        <v>545</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="122" t="s">
         <v>26</v>
       </c>
@@ -22096,67 +22019,63 @@
         <v>53</v>
       </c>
       <c r="D23" s="104">
-        <f t="shared" ref="D23:R23" ca="1" si="65">D22-D21</f>
-        <v>54</v>
+        <f t="shared" ref="D23:Q23" ca="1" si="61">D22-D21</f>
+        <v>28</v>
       </c>
       <c r="E23" s="104">
-        <f t="shared" ca="1" si="65"/>
-        <v>44</v>
+        <f t="shared" ca="1" si="61"/>
+        <v>35</v>
       </c>
       <c r="F23" s="104">
-        <f t="shared" ca="1" si="65"/>
-        <v>48</v>
+        <f t="shared" ca="1" si="61"/>
+        <v>32</v>
       </c>
       <c r="G23" s="104">
-        <f t="shared" ca="1" si="65"/>
-        <v>21</v>
+        <f t="shared" ca="1" si="61"/>
+        <v>45</v>
       </c>
       <c r="H23" s="104">
-        <f t="shared" ca="1" si="65"/>
-        <v>41</v>
+        <f t="shared" ca="1" si="61"/>
+        <v>60</v>
       </c>
       <c r="I23" s="104">
-        <f t="shared" ca="1" si="65"/>
-        <v>42</v>
+        <f t="shared" ca="1" si="61"/>
+        <v>20</v>
       </c>
       <c r="J23" s="104">
-        <f t="shared" ca="1" si="65"/>
-        <v>32</v>
+        <f t="shared" ca="1" si="61"/>
+        <v>35</v>
       </c>
       <c r="K23" s="104">
-        <f t="shared" ca="1" si="65"/>
-        <v>42</v>
+        <f t="shared" ca="1" si="61"/>
+        <v>56</v>
       </c>
       <c r="L23" s="104">
-        <f t="shared" ca="1" si="65"/>
-        <v>21</v>
+        <f t="shared" ca="1" si="61"/>
+        <v>39</v>
       </c>
       <c r="M23" s="104">
-        <f t="shared" ca="1" si="65"/>
-        <v>56</v>
+        <f t="shared" ca="1" si="61"/>
+        <v>22</v>
       </c>
       <c r="N23" s="104">
-        <f t="shared" ca="1" si="65"/>
-        <v>32</v>
+        <f t="shared" ca="1" si="61"/>
+        <v>28</v>
       </c>
       <c r="O23" s="104">
-        <f t="shared" ca="1" si="65"/>
-        <v>37</v>
+        <f t="shared" ca="1" si="61"/>
+        <v>23</v>
       </c>
       <c r="P23" s="104">
-        <f t="shared" ca="1" si="65"/>
-        <v>31</v>
+        <f t="shared" ca="1" si="61"/>
+        <v>40</v>
       </c>
       <c r="Q23" s="104">
-        <f t="shared" ca="1" si="65"/>
-        <v>24</v>
-      </c>
-      <c r="R23" s="104">
-        <f t="shared" ca="1" si="65"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="61"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="122" t="s">
         <v>26</v>
       </c>
@@ -22208,11 +22127,8 @@
       <c r="Q24" s="104">
         <v>500</v>
       </c>
-      <c r="R24" s="104">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="122" t="s">
         <v>26</v>
       </c>
@@ -22224,66 +22140,62 @@
       </c>
       <c r="D25" s="104">
         <f ca="1">RANDBETWEEN(20,60)+D24</f>
+        <v>524</v>
+      </c>
+      <c r="E25" s="104">
+        <f t="shared" ref="E25" ca="1" si="62">RANDBETWEEN(20,60)+E24</f>
+        <v>530</v>
+      </c>
+      <c r="F25" s="104">
+        <f t="shared" ref="F25" ca="1" si="63">RANDBETWEEN(20,60)+F24</f>
+        <v>553</v>
+      </c>
+      <c r="G25" s="104">
+        <f t="shared" ref="G25" ca="1" si="64">RANDBETWEEN(20,60)+G24</f>
+        <v>560</v>
+      </c>
+      <c r="H25" s="104">
+        <f t="shared" ref="H25" ca="1" si="65">RANDBETWEEN(20,60)+H24</f>
+        <v>552</v>
+      </c>
+      <c r="I25" s="104">
+        <f t="shared" ref="I25" ca="1" si="66">RANDBETWEEN(20,60)+I24</f>
+        <v>526</v>
+      </c>
+      <c r="J25" s="104">
+        <f t="shared" ref="J25" ca="1" si="67">RANDBETWEEN(20,60)+J24</f>
+        <v>546</v>
+      </c>
+      <c r="K25" s="104">
+        <f t="shared" ref="K25" ca="1" si="68">RANDBETWEEN(20,60)+K24</f>
+        <v>555</v>
+      </c>
+      <c r="L25" s="104">
+        <f t="shared" ref="L25" ca="1" si="69">RANDBETWEEN(20,60)+L24</f>
+        <v>549</v>
+      </c>
+      <c r="M25" s="104">
+        <f t="shared" ref="M25" ca="1" si="70">RANDBETWEEN(20,60)+M24</f>
+        <v>532</v>
+      </c>
+      <c r="N25" s="104">
+        <f t="shared" ref="N25" ca="1" si="71">RANDBETWEEN(20,60)+N24</f>
         <v>551</v>
       </c>
-      <c r="E25" s="104">
-        <f t="shared" ref="E25" ca="1" si="66">RANDBETWEEN(20,60)+E24</f>
-        <v>538</v>
-      </c>
-      <c r="F25" s="104">
-        <f t="shared" ref="F25" ca="1" si="67">RANDBETWEEN(20,60)+F24</f>
-        <v>537</v>
-      </c>
-      <c r="G25" s="104">
-        <f t="shared" ref="G25" ca="1" si="68">RANDBETWEEN(20,60)+G24</f>
-        <v>521</v>
-      </c>
-      <c r="H25" s="104">
-        <f t="shared" ref="H25" ca="1" si="69">RANDBETWEEN(20,60)+H24</f>
-        <v>547</v>
-      </c>
-      <c r="I25" s="104">
-        <f t="shared" ref="I25" ca="1" si="70">RANDBETWEEN(20,60)+I24</f>
-        <v>524</v>
-      </c>
-      <c r="J25" s="104">
-        <f t="shared" ref="J25" ca="1" si="71">RANDBETWEEN(20,60)+J24</f>
-        <v>554</v>
-      </c>
-      <c r="K25" s="104">
-        <f t="shared" ref="K25" ca="1" si="72">RANDBETWEEN(20,60)+K24</f>
-        <v>535</v>
-      </c>
-      <c r="L25" s="104">
-        <f t="shared" ref="L25" ca="1" si="73">RANDBETWEEN(20,60)+L24</f>
-        <v>552</v>
-      </c>
-      <c r="M25" s="104">
-        <f t="shared" ref="M25" ca="1" si="74">RANDBETWEEN(20,60)+M24</f>
-        <v>533</v>
-      </c>
-      <c r="N25" s="104">
-        <f t="shared" ref="N25" ca="1" si="75">RANDBETWEEN(20,60)+N24</f>
-        <v>532</v>
-      </c>
       <c r="O25" s="104">
-        <f t="shared" ref="O25" ca="1" si="76">RANDBETWEEN(20,60)+O24</f>
-        <v>560</v>
+        <f t="shared" ref="O25" ca="1" si="72">RANDBETWEEN(20,60)+O24</f>
+        <v>531</v>
       </c>
       <c r="P25" s="104">
-        <f t="shared" ref="P25" ca="1" si="77">RANDBETWEEN(20,60)+P24</f>
-        <v>530</v>
+        <f t="shared" ref="P25" ca="1" si="73">RANDBETWEEN(20,60)+P24</f>
+        <v>556</v>
       </c>
       <c r="Q25" s="104">
-        <f t="shared" ref="Q25" ca="1" si="78">RANDBETWEEN(20,60)+Q24</f>
-        <v>556</v>
-      </c>
-      <c r="R25" s="104">
-        <f t="shared" ref="R25" ca="1" si="79">RANDBETWEEN(20,60)+R24</f>
-        <v>525</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" ref="Q25" ca="1" si="74">RANDBETWEEN(20,60)+Q24</f>
+        <v>546</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="122" t="s">
         <v>26</v>
       </c>
@@ -22294,67 +22206,63 @@
         <v>53</v>
       </c>
       <c r="D26" s="104">
-        <f t="shared" ref="D26:R26" ca="1" si="80">D25-D24</f>
+        <f t="shared" ref="D26:Q26" ca="1" si="75">D25-D24</f>
+        <v>24</v>
+      </c>
+      <c r="E26" s="104">
+        <f t="shared" ca="1" si="75"/>
+        <v>30</v>
+      </c>
+      <c r="F26" s="104">
+        <f t="shared" ca="1" si="75"/>
+        <v>53</v>
+      </c>
+      <c r="G26" s="104">
+        <f t="shared" ca="1" si="75"/>
+        <v>60</v>
+      </c>
+      <c r="H26" s="104">
+        <f t="shared" ca="1" si="75"/>
+        <v>52</v>
+      </c>
+      <c r="I26" s="104">
+        <f t="shared" ca="1" si="75"/>
+        <v>26</v>
+      </c>
+      <c r="J26" s="104">
+        <f t="shared" ca="1" si="75"/>
+        <v>46</v>
+      </c>
+      <c r="K26" s="104">
+        <f t="shared" ca="1" si="75"/>
+        <v>55</v>
+      </c>
+      <c r="L26" s="104">
+        <f t="shared" ca="1" si="75"/>
+        <v>49</v>
+      </c>
+      <c r="M26" s="104">
+        <f t="shared" ca="1" si="75"/>
+        <v>32</v>
+      </c>
+      <c r="N26" s="104">
+        <f t="shared" ca="1" si="75"/>
         <v>51</v>
       </c>
-      <c r="E26" s="104">
-        <f t="shared" ca="1" si="80"/>
-        <v>38</v>
-      </c>
-      <c r="F26" s="104">
-        <f t="shared" ca="1" si="80"/>
-        <v>37</v>
-      </c>
-      <c r="G26" s="104">
-        <f t="shared" ca="1" si="80"/>
-        <v>21</v>
-      </c>
-      <c r="H26" s="104">
-        <f t="shared" ca="1" si="80"/>
-        <v>47</v>
-      </c>
-      <c r="I26" s="104">
-        <f t="shared" ca="1" si="80"/>
-        <v>24</v>
-      </c>
-      <c r="J26" s="104">
-        <f t="shared" ca="1" si="80"/>
-        <v>54</v>
-      </c>
-      <c r="K26" s="104">
-        <f t="shared" ca="1" si="80"/>
-        <v>35</v>
-      </c>
-      <c r="L26" s="104">
-        <f t="shared" ca="1" si="80"/>
-        <v>52</v>
-      </c>
-      <c r="M26" s="104">
-        <f t="shared" ca="1" si="80"/>
-        <v>33</v>
-      </c>
-      <c r="N26" s="104">
-        <f t="shared" ca="1" si="80"/>
-        <v>32</v>
-      </c>
       <c r="O26" s="104">
-        <f t="shared" ca="1" si="80"/>
-        <v>60</v>
+        <f t="shared" ca="1" si="75"/>
+        <v>31</v>
       </c>
       <c r="P26" s="104">
-        <f t="shared" ca="1" si="80"/>
-        <v>30</v>
+        <f t="shared" ca="1" si="75"/>
+        <v>56</v>
       </c>
       <c r="Q26" s="104">
-        <f t="shared" ca="1" si="80"/>
-        <v>56</v>
-      </c>
-      <c r="R26" s="104">
-        <f t="shared" ca="1" si="80"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="75"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="122" t="s">
         <v>26</v>
       </c>
@@ -22406,11 +22314,8 @@
       <c r="Q27" s="104">
         <v>500</v>
       </c>
-      <c r="R27" s="104">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="122" t="s">
         <v>26</v>
       </c>
@@ -22425,63 +22330,59 @@
         <v>542</v>
       </c>
       <c r="E28" s="104">
-        <f t="shared" ref="E28" ca="1" si="81">RANDBETWEEN(20,60)+E27</f>
-        <v>526</v>
+        <f t="shared" ref="E28" ca="1" si="76">RANDBETWEEN(20,60)+E27</f>
+        <v>547</v>
       </c>
       <c r="F28" s="104">
-        <f t="shared" ref="F28" ca="1" si="82">RANDBETWEEN(20,60)+F27</f>
-        <v>532</v>
+        <f t="shared" ref="F28" ca="1" si="77">RANDBETWEEN(20,60)+F27</f>
+        <v>539</v>
       </c>
       <c r="G28" s="104">
-        <f t="shared" ref="G28" ca="1" si="83">RANDBETWEEN(20,60)+G27</f>
-        <v>556</v>
+        <f t="shared" ref="G28" ca="1" si="78">RANDBETWEEN(20,60)+G27</f>
+        <v>528</v>
       </c>
       <c r="H28" s="104">
-        <f t="shared" ref="H28" ca="1" si="84">RANDBETWEEN(20,60)+H27</f>
+        <f t="shared" ref="H28" ca="1" si="79">RANDBETWEEN(20,60)+H27</f>
+        <v>540</v>
+      </c>
+      <c r="I28" s="104">
+        <f t="shared" ref="I28" ca="1" si="80">RANDBETWEEN(20,60)+I27</f>
+        <v>543</v>
+      </c>
+      <c r="J28" s="104">
+        <f t="shared" ref="J28" ca="1" si="81">RANDBETWEEN(20,60)+J27</f>
+        <v>529</v>
+      </c>
+      <c r="K28" s="104">
+        <f t="shared" ref="K28" ca="1" si="82">RANDBETWEEN(20,60)+K27</f>
+        <v>539</v>
+      </c>
+      <c r="L28" s="104">
+        <f t="shared" ref="L28" ca="1" si="83">RANDBETWEEN(20,60)+L27</f>
+        <v>553</v>
+      </c>
+      <c r="M28" s="104">
+        <f t="shared" ref="M28" ca="1" si="84">RANDBETWEEN(20,60)+M27</f>
+        <v>552</v>
+      </c>
+      <c r="N28" s="104">
+        <f t="shared" ref="N28" ca="1" si="85">RANDBETWEEN(20,60)+N27</f>
+        <v>521</v>
+      </c>
+      <c r="O28" s="104">
+        <f t="shared" ref="O28" ca="1" si="86">RANDBETWEEN(20,60)+O27</f>
+        <v>547</v>
+      </c>
+      <c r="P28" s="104">
+        <f t="shared" ref="P28" ca="1" si="87">RANDBETWEEN(20,60)+P27</f>
+        <v>547</v>
+      </c>
+      <c r="Q28" s="104">
+        <f t="shared" ref="Q28" ca="1" si="88">RANDBETWEEN(20,60)+Q27</f>
         <v>531</v>
       </c>
-      <c r="I28" s="104">
-        <f t="shared" ref="I28" ca="1" si="85">RANDBETWEEN(20,60)+I27</f>
-        <v>522</v>
-      </c>
-      <c r="J28" s="104">
-        <f t="shared" ref="J28" ca="1" si="86">RANDBETWEEN(20,60)+J27</f>
-        <v>529</v>
-      </c>
-      <c r="K28" s="104">
-        <f t="shared" ref="K28" ca="1" si="87">RANDBETWEEN(20,60)+K27</f>
-        <v>535</v>
-      </c>
-      <c r="L28" s="104">
-        <f t="shared" ref="L28" ca="1" si="88">RANDBETWEEN(20,60)+L27</f>
-        <v>527</v>
-      </c>
-      <c r="M28" s="104">
-        <f t="shared" ref="M28" ca="1" si="89">RANDBETWEEN(20,60)+M27</f>
-        <v>534</v>
-      </c>
-      <c r="N28" s="104">
-        <f t="shared" ref="N28" ca="1" si="90">RANDBETWEEN(20,60)+N27</f>
-        <v>538</v>
-      </c>
-      <c r="O28" s="104">
-        <f t="shared" ref="O28" ca="1" si="91">RANDBETWEEN(20,60)+O27</f>
-        <v>523</v>
-      </c>
-      <c r="P28" s="104">
-        <f t="shared" ref="P28" ca="1" si="92">RANDBETWEEN(20,60)+P27</f>
-        <v>554</v>
-      </c>
-      <c r="Q28" s="104">
-        <f t="shared" ref="Q28" ca="1" si="93">RANDBETWEEN(20,60)+Q27</f>
-        <v>529</v>
-      </c>
-      <c r="R28" s="104">
-        <f t="shared" ref="R28" ca="1" si="94">RANDBETWEEN(20,60)+R27</f>
-        <v>521</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="122" t="s">
         <v>26</v>
       </c>
@@ -22492,67 +22393,63 @@
         <v>53</v>
       </c>
       <c r="D29" s="104">
-        <f t="shared" ref="D29:R29" ca="1" si="95">D28-D27</f>
+        <f t="shared" ref="D29:Q29" ca="1" si="89">D28-D27</f>
         <v>42</v>
       </c>
       <c r="E29" s="104">
-        <f t="shared" ca="1" si="95"/>
-        <v>26</v>
+        <f t="shared" ca="1" si="89"/>
+        <v>47</v>
       </c>
       <c r="F29" s="104">
-        <f t="shared" ca="1" si="95"/>
-        <v>32</v>
+        <f t="shared" ca="1" si="89"/>
+        <v>39</v>
       </c>
       <c r="G29" s="104">
-        <f t="shared" ca="1" si="95"/>
-        <v>56</v>
+        <f t="shared" ca="1" si="89"/>
+        <v>28</v>
       </c>
       <c r="H29" s="104">
-        <f t="shared" ca="1" si="95"/>
+        <f t="shared" ca="1" si="89"/>
+        <v>40</v>
+      </c>
+      <c r="I29" s="104">
+        <f t="shared" ca="1" si="89"/>
+        <v>43</v>
+      </c>
+      <c r="J29" s="104">
+        <f t="shared" ca="1" si="89"/>
+        <v>29</v>
+      </c>
+      <c r="K29" s="104">
+        <f t="shared" ca="1" si="89"/>
+        <v>39</v>
+      </c>
+      <c r="L29" s="104">
+        <f t="shared" ca="1" si="89"/>
+        <v>53</v>
+      </c>
+      <c r="M29" s="104">
+        <f t="shared" ca="1" si="89"/>
+        <v>52</v>
+      </c>
+      <c r="N29" s="104">
+        <f t="shared" ca="1" si="89"/>
+        <v>21</v>
+      </c>
+      <c r="O29" s="104">
+        <f t="shared" ca="1" si="89"/>
+        <v>47</v>
+      </c>
+      <c r="P29" s="104">
+        <f t="shared" ca="1" si="89"/>
+        <v>47</v>
+      </c>
+      <c r="Q29" s="104">
+        <f t="shared" ca="1" si="89"/>
         <v>31</v>
       </c>
-      <c r="I29" s="104">
-        <f t="shared" ca="1" si="95"/>
-        <v>22</v>
-      </c>
-      <c r="J29" s="104">
-        <f t="shared" ca="1" si="95"/>
-        <v>29</v>
-      </c>
-      <c r="K29" s="104">
-        <f t="shared" ca="1" si="95"/>
-        <v>35</v>
-      </c>
-      <c r="L29" s="104">
-        <f t="shared" ca="1" si="95"/>
-        <v>27</v>
-      </c>
-      <c r="M29" s="104">
-        <f t="shared" ca="1" si="95"/>
-        <v>34</v>
-      </c>
-      <c r="N29" s="104">
-        <f t="shared" ca="1" si="95"/>
-        <v>38</v>
-      </c>
-      <c r="O29" s="104">
-        <f t="shared" ca="1" si="95"/>
-        <v>23</v>
-      </c>
-      <c r="P29" s="104">
-        <f t="shared" ca="1" si="95"/>
-        <v>54</v>
-      </c>
-      <c r="Q29" s="104">
-        <f t="shared" ca="1" si="95"/>
-        <v>29</v>
-      </c>
-      <c r="R29" s="104">
-        <f t="shared" ca="1" si="95"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="122" t="s">
         <v>26</v>
       </c>
@@ -22604,11 +22501,8 @@
       <c r="Q30" s="104">
         <v>500</v>
       </c>
-      <c r="R30" s="104">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="122" t="s">
         <v>26</v>
       </c>
@@ -22620,66 +22514,62 @@
       </c>
       <c r="D31" s="104">
         <f ca="1">RANDBETWEEN(20,60)+D30</f>
-        <v>555</v>
+        <v>540</v>
       </c>
       <c r="E31" s="104">
-        <f t="shared" ref="E31" ca="1" si="96">RANDBETWEEN(20,60)+E30</f>
-        <v>559</v>
+        <f t="shared" ref="E31" ca="1" si="90">RANDBETWEEN(20,60)+E30</f>
+        <v>541</v>
       </c>
       <c r="F31" s="104">
-        <f t="shared" ref="F31" ca="1" si="97">RANDBETWEEN(20,60)+F30</f>
-        <v>554</v>
+        <f t="shared" ref="F31" ca="1" si="91">RANDBETWEEN(20,60)+F30</f>
+        <v>541</v>
       </c>
       <c r="G31" s="104">
-        <f t="shared" ref="G31" ca="1" si="98">RANDBETWEEN(20,60)+G30</f>
+        <f t="shared" ref="G31" ca="1" si="92">RANDBETWEEN(20,60)+G30</f>
+        <v>538</v>
+      </c>
+      <c r="H31" s="104">
+        <f t="shared" ref="H31" ca="1" si="93">RANDBETWEEN(20,60)+H30</f>
+        <v>560</v>
+      </c>
+      <c r="I31" s="104">
+        <f t="shared" ref="I31" ca="1" si="94">RANDBETWEEN(20,60)+I30</f>
+        <v>541</v>
+      </c>
+      <c r="J31" s="104">
+        <f t="shared" ref="J31" ca="1" si="95">RANDBETWEEN(20,60)+J30</f>
+        <v>542</v>
+      </c>
+      <c r="K31" s="104">
+        <f t="shared" ref="K31" ca="1" si="96">RANDBETWEEN(20,60)+K30</f>
+        <v>534</v>
+      </c>
+      <c r="L31" s="104">
+        <f t="shared" ref="L31" ca="1" si="97">RANDBETWEEN(20,60)+L30</f>
+        <v>530</v>
+      </c>
+      <c r="M31" s="104">
+        <f t="shared" ref="M31" ca="1" si="98">RANDBETWEEN(20,60)+M30</f>
+        <v>546</v>
+      </c>
+      <c r="N31" s="104">
+        <f t="shared" ref="N31" ca="1" si="99">RANDBETWEEN(20,60)+N30</f>
         <v>536</v>
       </c>
-      <c r="H31" s="104">
-        <f t="shared" ref="H31" ca="1" si="99">RANDBETWEEN(20,60)+H30</f>
-        <v>522</v>
-      </c>
-      <c r="I31" s="104">
-        <f t="shared" ref="I31" ca="1" si="100">RANDBETWEEN(20,60)+I30</f>
-        <v>531</v>
-      </c>
-      <c r="J31" s="104">
-        <f t="shared" ref="J31" ca="1" si="101">RANDBETWEEN(20,60)+J30</f>
-        <v>543</v>
-      </c>
-      <c r="K31" s="104">
-        <f t="shared" ref="K31" ca="1" si="102">RANDBETWEEN(20,60)+K30</f>
-        <v>536</v>
-      </c>
-      <c r="L31" s="104">
-        <f t="shared" ref="L31" ca="1" si="103">RANDBETWEEN(20,60)+L30</f>
-        <v>541</v>
-      </c>
-      <c r="M31" s="104">
-        <f t="shared" ref="M31" ca="1" si="104">RANDBETWEEN(20,60)+M30</f>
-        <v>520</v>
-      </c>
-      <c r="N31" s="104">
-        <f t="shared" ref="N31" ca="1" si="105">RANDBETWEEN(20,60)+N30</f>
-        <v>552</v>
-      </c>
       <c r="O31" s="104">
-        <f t="shared" ref="O31" ca="1" si="106">RANDBETWEEN(20,60)+O30</f>
-        <v>556</v>
+        <f t="shared" ref="O31" ca="1" si="100">RANDBETWEEN(20,60)+O30</f>
+        <v>538</v>
       </c>
       <c r="P31" s="104">
-        <f t="shared" ref="P31" ca="1" si="107">RANDBETWEEN(20,60)+P30</f>
-        <v>526</v>
+        <f t="shared" ref="P31" ca="1" si="101">RANDBETWEEN(20,60)+P30</f>
+        <v>530</v>
       </c>
       <c r="Q31" s="104">
-        <f t="shared" ref="Q31" ca="1" si="108">RANDBETWEEN(20,60)+Q30</f>
-        <v>553</v>
-      </c>
-      <c r="R31" s="104">
-        <f t="shared" ref="R31" ca="1" si="109">RANDBETWEEN(20,60)+R30</f>
-        <v>533</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" ref="Q31" ca="1" si="102">RANDBETWEEN(20,60)+Q30</f>
+        <v>523</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="122" t="s">
         <v>26</v>
       </c>
@@ -22690,67 +22580,63 @@
         <v>53</v>
       </c>
       <c r="D32" s="104">
-        <f t="shared" ref="D32:R32" ca="1" si="110">D31-D30</f>
-        <v>55</v>
+        <f t="shared" ref="D32:Q32" ca="1" si="103">D31-D30</f>
+        <v>40</v>
       </c>
       <c r="E32" s="104">
-        <f t="shared" ca="1" si="110"/>
-        <v>59</v>
+        <f t="shared" ca="1" si="103"/>
+        <v>41</v>
       </c>
       <c r="F32" s="104">
-        <f t="shared" ca="1" si="110"/>
-        <v>54</v>
+        <f t="shared" ca="1" si="103"/>
+        <v>41</v>
       </c>
       <c r="G32" s="104">
-        <f t="shared" ca="1" si="110"/>
+        <f t="shared" ca="1" si="103"/>
+        <v>38</v>
+      </c>
+      <c r="H32" s="104">
+        <f t="shared" ca="1" si="103"/>
+        <v>60</v>
+      </c>
+      <c r="I32" s="104">
+        <f t="shared" ca="1" si="103"/>
+        <v>41</v>
+      </c>
+      <c r="J32" s="104">
+        <f t="shared" ca="1" si="103"/>
+        <v>42</v>
+      </c>
+      <c r="K32" s="104">
+        <f t="shared" ca="1" si="103"/>
+        <v>34</v>
+      </c>
+      <c r="L32" s="104">
+        <f t="shared" ca="1" si="103"/>
+        <v>30</v>
+      </c>
+      <c r="M32" s="104">
+        <f t="shared" ca="1" si="103"/>
+        <v>46</v>
+      </c>
+      <c r="N32" s="104">
+        <f t="shared" ca="1" si="103"/>
         <v>36</v>
       </c>
-      <c r="H32" s="104">
-        <f t="shared" ca="1" si="110"/>
-        <v>22</v>
-      </c>
-      <c r="I32" s="104">
-        <f t="shared" ca="1" si="110"/>
-        <v>31</v>
-      </c>
-      <c r="J32" s="104">
-        <f t="shared" ca="1" si="110"/>
-        <v>43</v>
-      </c>
-      <c r="K32" s="104">
-        <f t="shared" ca="1" si="110"/>
-        <v>36</v>
-      </c>
-      <c r="L32" s="104">
-        <f t="shared" ca="1" si="110"/>
-        <v>41</v>
-      </c>
-      <c r="M32" s="104">
-        <f t="shared" ca="1" si="110"/>
-        <v>20</v>
-      </c>
-      <c r="N32" s="104">
-        <f t="shared" ca="1" si="110"/>
-        <v>52</v>
-      </c>
       <c r="O32" s="104">
-        <f t="shared" ca="1" si="110"/>
-        <v>56</v>
+        <f t="shared" ca="1" si="103"/>
+        <v>38</v>
       </c>
       <c r="P32" s="104">
-        <f t="shared" ca="1" si="110"/>
-        <v>26</v>
+        <f t="shared" ca="1" si="103"/>
+        <v>30</v>
       </c>
       <c r="Q32" s="104">
-        <f t="shared" ca="1" si="110"/>
-        <v>53</v>
-      </c>
-      <c r="R32" s="104">
-        <f t="shared" ca="1" si="110"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="103"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="123" t="s">
         <v>32</v>
       </c>
@@ -22802,11 +22688,8 @@
       <c r="Q33" s="105">
         <v>500</v>
       </c>
-      <c r="R33" s="105">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="123" t="s">
         <v>32</v>
       </c>
@@ -22818,66 +22701,62 @@
       </c>
       <c r="D34" s="105">
         <f ca="1">RANDBETWEEN(20,60)+D33</f>
+        <v>549</v>
+      </c>
+      <c r="E34" s="105">
+        <f t="shared" ref="E34" ca="1" si="104">RANDBETWEEN(20,60)+E33</f>
+        <v>534</v>
+      </c>
+      <c r="F34" s="105">
+        <f t="shared" ref="F34" ca="1" si="105">RANDBETWEEN(20,60)+F33</f>
+        <v>529</v>
+      </c>
+      <c r="G34" s="105">
+        <f t="shared" ref="G34" ca="1" si="106">RANDBETWEEN(20,60)+G33</f>
+        <v>553</v>
+      </c>
+      <c r="H34" s="105">
+        <f t="shared" ref="H34" ca="1" si="107">RANDBETWEEN(20,60)+H33</f>
+        <v>538</v>
+      </c>
+      <c r="I34" s="105">
+        <f t="shared" ref="I34" ca="1" si="108">RANDBETWEEN(20,60)+I33</f>
+        <v>529</v>
+      </c>
+      <c r="J34" s="105">
+        <f t="shared" ref="J34" ca="1" si="109">RANDBETWEEN(20,60)+J33</f>
+        <v>536</v>
+      </c>
+      <c r="K34" s="105">
+        <f t="shared" ref="K34" ca="1" si="110">RANDBETWEEN(20,60)+K33</f>
+        <v>542</v>
+      </c>
+      <c r="L34" s="105">
+        <f t="shared" ref="L34" ca="1" si="111">RANDBETWEEN(20,60)+L33</f>
         <v>544</v>
       </c>
-      <c r="E34" s="105">
-        <f t="shared" ref="E34" ca="1" si="111">RANDBETWEEN(20,60)+E33</f>
-        <v>523</v>
-      </c>
-      <c r="F34" s="105">
-        <f t="shared" ref="F34" ca="1" si="112">RANDBETWEEN(20,60)+F33</f>
-        <v>557</v>
-      </c>
-      <c r="G34" s="105">
-        <f t="shared" ref="G34" ca="1" si="113">RANDBETWEEN(20,60)+G33</f>
-        <v>532</v>
-      </c>
-      <c r="H34" s="105">
-        <f t="shared" ref="H34" ca="1" si="114">RANDBETWEEN(20,60)+H33</f>
-        <v>530</v>
-      </c>
-      <c r="I34" s="105">
-        <f t="shared" ref="I34" ca="1" si="115">RANDBETWEEN(20,60)+I33</f>
-        <v>560</v>
-      </c>
-      <c r="J34" s="105">
-        <f t="shared" ref="J34" ca="1" si="116">RANDBETWEEN(20,60)+J33</f>
-        <v>557</v>
-      </c>
-      <c r="K34" s="105">
-        <f t="shared" ref="K34" ca="1" si="117">RANDBETWEEN(20,60)+K33</f>
-        <v>546</v>
-      </c>
-      <c r="L34" s="105">
-        <f t="shared" ref="L34" ca="1" si="118">RANDBETWEEN(20,60)+L33</f>
-        <v>530</v>
-      </c>
       <c r="M34" s="105">
-        <f t="shared" ref="M34" ca="1" si="119">RANDBETWEEN(20,60)+M33</f>
+        <f t="shared" ref="M34" ca="1" si="112">RANDBETWEEN(20,60)+M33</f>
+        <v>550</v>
+      </c>
+      <c r="N34" s="105">
+        <f t="shared" ref="N34" ca="1" si="113">RANDBETWEEN(20,60)+N33</f>
+        <v>531</v>
+      </c>
+      <c r="O34" s="105">
+        <f t="shared" ref="O34" ca="1" si="114">RANDBETWEEN(20,60)+O33</f>
+        <v>547</v>
+      </c>
+      <c r="P34" s="105">
+        <f t="shared" ref="P34" ca="1" si="115">RANDBETWEEN(20,60)+P33</f>
         <v>558</v>
       </c>
-      <c r="N34" s="105">
-        <f t="shared" ref="N34" ca="1" si="120">RANDBETWEEN(20,60)+N33</f>
-        <v>539</v>
-      </c>
-      <c r="O34" s="105">
-        <f t="shared" ref="O34" ca="1" si="121">RANDBETWEEN(20,60)+O33</f>
+      <c r="Q34" s="105">
+        <f t="shared" ref="Q34" ca="1" si="116">RANDBETWEEN(20,60)+Q33</f>
         <v>529</v>
       </c>
-      <c r="P34" s="105">
-        <f t="shared" ref="P34" ca="1" si="122">RANDBETWEEN(20,60)+P33</f>
-        <v>535</v>
-      </c>
-      <c r="Q34" s="105">
-        <f t="shared" ref="Q34" ca="1" si="123">RANDBETWEEN(20,60)+Q33</f>
-        <v>535</v>
-      </c>
-      <c r="R34" s="105">
-        <f t="shared" ref="R34" ca="1" si="124">RANDBETWEEN(20,60)+R33</f>
-        <v>544</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="123" t="s">
         <v>32</v>
       </c>
@@ -22888,67 +22767,63 @@
         <v>53</v>
       </c>
       <c r="D35" s="105">
-        <f t="shared" ref="D35:R35" ca="1" si="125">D34-D33</f>
+        <f t="shared" ref="D35:Q35" ca="1" si="117">D34-D33</f>
+        <v>49</v>
+      </c>
+      <c r="E35" s="105">
+        <f t="shared" ca="1" si="117"/>
+        <v>34</v>
+      </c>
+      <c r="F35" s="105">
+        <f t="shared" ca="1" si="117"/>
+        <v>29</v>
+      </c>
+      <c r="G35" s="105">
+        <f t="shared" ca="1" si="117"/>
+        <v>53</v>
+      </c>
+      <c r="H35" s="105">
+        <f t="shared" ca="1" si="117"/>
+        <v>38</v>
+      </c>
+      <c r="I35" s="105">
+        <f t="shared" ca="1" si="117"/>
+        <v>29</v>
+      </c>
+      <c r="J35" s="105">
+        <f t="shared" ca="1" si="117"/>
+        <v>36</v>
+      </c>
+      <c r="K35" s="105">
+        <f t="shared" ca="1" si="117"/>
+        <v>42</v>
+      </c>
+      <c r="L35" s="105">
+        <f t="shared" ca="1" si="117"/>
         <v>44</v>
       </c>
-      <c r="E35" s="105">
-        <f t="shared" ca="1" si="125"/>
-        <v>23</v>
-      </c>
-      <c r="F35" s="105">
-        <f t="shared" ca="1" si="125"/>
-        <v>57</v>
-      </c>
-      <c r="G35" s="105">
-        <f t="shared" ca="1" si="125"/>
-        <v>32</v>
-      </c>
-      <c r="H35" s="105">
-        <f t="shared" ca="1" si="125"/>
-        <v>30</v>
-      </c>
-      <c r="I35" s="105">
-        <f t="shared" ca="1" si="125"/>
-        <v>60</v>
-      </c>
-      <c r="J35" s="105">
-        <f t="shared" ca="1" si="125"/>
-        <v>57</v>
-      </c>
-      <c r="K35" s="105">
-        <f t="shared" ca="1" si="125"/>
-        <v>46</v>
-      </c>
-      <c r="L35" s="105">
-        <f t="shared" ca="1" si="125"/>
-        <v>30</v>
-      </c>
       <c r="M35" s="105">
-        <f t="shared" ca="1" si="125"/>
+        <f t="shared" ca="1" si="117"/>
+        <v>50</v>
+      </c>
+      <c r="N35" s="105">
+        <f t="shared" ca="1" si="117"/>
+        <v>31</v>
+      </c>
+      <c r="O35" s="105">
+        <f t="shared" ca="1" si="117"/>
+        <v>47</v>
+      </c>
+      <c r="P35" s="105">
+        <f t="shared" ca="1" si="117"/>
         <v>58</v>
       </c>
-      <c r="N35" s="105">
-        <f t="shared" ca="1" si="125"/>
-        <v>39</v>
-      </c>
-      <c r="O35" s="105">
-        <f t="shared" ca="1" si="125"/>
+      <c r="Q35" s="105">
+        <f t="shared" ca="1" si="117"/>
         <v>29</v>
       </c>
-      <c r="P35" s="105">
-        <f t="shared" ca="1" si="125"/>
-        <v>35</v>
-      </c>
-      <c r="Q35" s="105">
-        <f t="shared" ca="1" si="125"/>
-        <v>35</v>
-      </c>
-      <c r="R35" s="105">
-        <f t="shared" ca="1" si="125"/>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="123" t="s">
         <v>32</v>
       </c>
@@ -23000,11 +22875,8 @@
       <c r="Q36" s="105">
         <v>500</v>
       </c>
-      <c r="R36" s="105">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="123" t="s">
         <v>32</v>
       </c>
@@ -23016,66 +22888,62 @@
       </c>
       <c r="D37" s="105">
         <f ca="1">RANDBETWEEN(20,60)+D36</f>
-        <v>550</v>
+        <v>526</v>
       </c>
       <c r="E37" s="105">
-        <f t="shared" ref="E37" ca="1" si="126">RANDBETWEEN(20,60)+E36</f>
-        <v>547</v>
+        <f t="shared" ref="E37" ca="1" si="118">RANDBETWEEN(20,60)+E36</f>
+        <v>557</v>
       </c>
       <c r="F37" s="105">
-        <f t="shared" ref="F37" ca="1" si="127">RANDBETWEEN(20,60)+F36</f>
-        <v>543</v>
+        <f t="shared" ref="F37" ca="1" si="119">RANDBETWEEN(20,60)+F36</f>
+        <v>545</v>
       </c>
       <c r="G37" s="105">
-        <f t="shared" ref="G37" ca="1" si="128">RANDBETWEEN(20,60)+G36</f>
-        <v>537</v>
+        <f t="shared" ref="G37" ca="1" si="120">RANDBETWEEN(20,60)+G36</f>
+        <v>540</v>
       </c>
       <c r="H37" s="105">
-        <f t="shared" ref="H37" ca="1" si="129">RANDBETWEEN(20,60)+H36</f>
+        <f t="shared" ref="H37" ca="1" si="121">RANDBETWEEN(20,60)+H36</f>
+        <v>545</v>
+      </c>
+      <c r="I37" s="105">
+        <f t="shared" ref="I37" ca="1" si="122">RANDBETWEEN(20,60)+I36</f>
+        <v>556</v>
+      </c>
+      <c r="J37" s="105">
+        <f t="shared" ref="J37" ca="1" si="123">RANDBETWEEN(20,60)+J36</f>
+        <v>544</v>
+      </c>
+      <c r="K37" s="105">
+        <f t="shared" ref="K37" ca="1" si="124">RANDBETWEEN(20,60)+K36</f>
+        <v>535</v>
+      </c>
+      <c r="L37" s="105">
+        <f t="shared" ref="L37" ca="1" si="125">RANDBETWEEN(20,60)+L36</f>
+        <v>541</v>
+      </c>
+      <c r="M37" s="105">
+        <f t="shared" ref="M37" ca="1" si="126">RANDBETWEEN(20,60)+M36</f>
+        <v>542</v>
+      </c>
+      <c r="N37" s="105">
+        <f t="shared" ref="N37" ca="1" si="127">RANDBETWEEN(20,60)+N36</f>
+        <v>551</v>
+      </c>
+      <c r="O37" s="105">
+        <f t="shared" ref="O37" ca="1" si="128">RANDBETWEEN(20,60)+O36</f>
+        <v>546</v>
+      </c>
+      <c r="P37" s="105">
+        <f t="shared" ref="P37" ca="1" si="129">RANDBETWEEN(20,60)+P36</f>
+        <v>558</v>
+      </c>
+      <c r="Q37" s="105">
+        <f t="shared" ref="Q37" ca="1" si="130">RANDBETWEEN(20,60)+Q36</f>
         <v>534</v>
       </c>
-      <c r="I37" s="105">
-        <f t="shared" ref="I37" ca="1" si="130">RANDBETWEEN(20,60)+I36</f>
-        <v>548</v>
-      </c>
-      <c r="J37" s="105">
-        <f t="shared" ref="J37" ca="1" si="131">RANDBETWEEN(20,60)+J36</f>
-        <v>540</v>
-      </c>
-      <c r="K37" s="105">
-        <f t="shared" ref="K37" ca="1" si="132">RANDBETWEEN(20,60)+K36</f>
-        <v>531</v>
-      </c>
-      <c r="L37" s="105">
-        <f t="shared" ref="L37" ca="1" si="133">RANDBETWEEN(20,60)+L36</f>
-        <v>540</v>
-      </c>
-      <c r="M37" s="105">
-        <f t="shared" ref="M37" ca="1" si="134">RANDBETWEEN(20,60)+M36</f>
-        <v>547</v>
-      </c>
-      <c r="N37" s="105">
-        <f t="shared" ref="N37" ca="1" si="135">RANDBETWEEN(20,60)+N36</f>
-        <v>541</v>
-      </c>
-      <c r="O37" s="105">
-        <f t="shared" ref="O37" ca="1" si="136">RANDBETWEEN(20,60)+O36</f>
-        <v>528</v>
-      </c>
-      <c r="P37" s="105">
-        <f t="shared" ref="P37" ca="1" si="137">RANDBETWEEN(20,60)+P36</f>
-        <v>535</v>
-      </c>
-      <c r="Q37" s="105">
-        <f t="shared" ref="Q37" ca="1" si="138">RANDBETWEEN(20,60)+Q36</f>
-        <v>543</v>
-      </c>
-      <c r="R37" s="105">
-        <f t="shared" ref="R37" ca="1" si="139">RANDBETWEEN(20,60)+R36</f>
-        <v>543</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="123" t="s">
         <v>32</v>
       </c>
@@ -23086,67 +22954,63 @@
         <v>53</v>
       </c>
       <c r="D38" s="105">
-        <f t="shared" ref="D38:R38" ca="1" si="140">D37-D36</f>
-        <v>50</v>
+        <f t="shared" ref="D38:Q38" ca="1" si="131">D37-D36</f>
+        <v>26</v>
       </c>
       <c r="E38" s="105">
-        <f t="shared" ca="1" si="140"/>
-        <v>47</v>
+        <f t="shared" ca="1" si="131"/>
+        <v>57</v>
       </c>
       <c r="F38" s="105">
-        <f t="shared" ca="1" si="140"/>
-        <v>43</v>
+        <f t="shared" ca="1" si="131"/>
+        <v>45</v>
       </c>
       <c r="G38" s="105">
-        <f t="shared" ca="1" si="140"/>
-        <v>37</v>
+        <f t="shared" ca="1" si="131"/>
+        <v>40</v>
       </c>
       <c r="H38" s="105">
-        <f t="shared" ca="1" si="140"/>
+        <f t="shared" ca="1" si="131"/>
+        <v>45</v>
+      </c>
+      <c r="I38" s="105">
+        <f t="shared" ca="1" si="131"/>
+        <v>56</v>
+      </c>
+      <c r="J38" s="105">
+        <f t="shared" ca="1" si="131"/>
+        <v>44</v>
+      </c>
+      <c r="K38" s="105">
+        <f t="shared" ca="1" si="131"/>
+        <v>35</v>
+      </c>
+      <c r="L38" s="105">
+        <f t="shared" ca="1" si="131"/>
+        <v>41</v>
+      </c>
+      <c r="M38" s="105">
+        <f t="shared" ca="1" si="131"/>
+        <v>42</v>
+      </c>
+      <c r="N38" s="105">
+        <f t="shared" ca="1" si="131"/>
+        <v>51</v>
+      </c>
+      <c r="O38" s="105">
+        <f t="shared" ca="1" si="131"/>
+        <v>46</v>
+      </c>
+      <c r="P38" s="105">
+        <f t="shared" ca="1" si="131"/>
+        <v>58</v>
+      </c>
+      <c r="Q38" s="105">
+        <f t="shared" ca="1" si="131"/>
         <v>34</v>
       </c>
-      <c r="I38" s="105">
-        <f t="shared" ca="1" si="140"/>
-        <v>48</v>
-      </c>
-      <c r="J38" s="105">
-        <f t="shared" ca="1" si="140"/>
-        <v>40</v>
-      </c>
-      <c r="K38" s="105">
-        <f t="shared" ca="1" si="140"/>
-        <v>31</v>
-      </c>
-      <c r="L38" s="105">
-        <f t="shared" ca="1" si="140"/>
-        <v>40</v>
-      </c>
-      <c r="M38" s="105">
-        <f t="shared" ca="1" si="140"/>
-        <v>47</v>
-      </c>
-      <c r="N38" s="105">
-        <f t="shared" ca="1" si="140"/>
-        <v>41</v>
-      </c>
-      <c r="O38" s="105">
-        <f t="shared" ca="1" si="140"/>
-        <v>28</v>
-      </c>
-      <c r="P38" s="105">
-        <f t="shared" ca="1" si="140"/>
-        <v>35</v>
-      </c>
-      <c r="Q38" s="105">
-        <f t="shared" ca="1" si="140"/>
-        <v>43</v>
-      </c>
-      <c r="R38" s="105">
-        <f t="shared" ca="1" si="140"/>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="123" t="s">
         <v>32</v>
       </c>
@@ -23198,11 +23062,8 @@
       <c r="Q39" s="105">
         <v>500</v>
       </c>
-      <c r="R39" s="105">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="123" t="s">
         <v>32</v>
       </c>
@@ -23214,66 +23075,62 @@
       </c>
       <c r="D40" s="105">
         <f ca="1">RANDBETWEEN(20,60)+D39</f>
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E40" s="105">
-        <f t="shared" ref="E40" ca="1" si="141">RANDBETWEEN(20,60)+E39</f>
-        <v>556</v>
+        <f t="shared" ref="E40" ca="1" si="132">RANDBETWEEN(20,60)+E39</f>
+        <v>530</v>
       </c>
       <c r="F40" s="105">
-        <f t="shared" ref="F40" ca="1" si="142">RANDBETWEEN(20,60)+F39</f>
-        <v>532</v>
+        <f t="shared" ref="F40" ca="1" si="133">RANDBETWEEN(20,60)+F39</f>
+        <v>523</v>
       </c>
       <c r="G40" s="105">
-        <f t="shared" ref="G40" ca="1" si="143">RANDBETWEEN(20,60)+G39</f>
+        <f t="shared" ref="G40" ca="1" si="134">RANDBETWEEN(20,60)+G39</f>
         <v>555</v>
       </c>
       <c r="H40" s="105">
-        <f t="shared" ref="H40" ca="1" si="144">RANDBETWEEN(20,60)+H39</f>
-        <v>533</v>
+        <f t="shared" ref="H40" ca="1" si="135">RANDBETWEEN(20,60)+H39</f>
+        <v>548</v>
       </c>
       <c r="I40" s="105">
-        <f t="shared" ref="I40" ca="1" si="145">RANDBETWEEN(20,60)+I39</f>
-        <v>557</v>
+        <f t="shared" ref="I40" ca="1" si="136">RANDBETWEEN(20,60)+I39</f>
+        <v>549</v>
       </c>
       <c r="J40" s="105">
-        <f t="shared" ref="J40" ca="1" si="146">RANDBETWEEN(20,60)+J39</f>
-        <v>533</v>
+        <f t="shared" ref="J40" ca="1" si="137">RANDBETWEEN(20,60)+J39</f>
+        <v>548</v>
       </c>
       <c r="K40" s="105">
-        <f t="shared" ref="K40" ca="1" si="147">RANDBETWEEN(20,60)+K39</f>
-        <v>547</v>
+        <f t="shared" ref="K40" ca="1" si="138">RANDBETWEEN(20,60)+K39</f>
+        <v>536</v>
       </c>
       <c r="L40" s="105">
-        <f t="shared" ref="L40" ca="1" si="148">RANDBETWEEN(20,60)+L39</f>
-        <v>543</v>
+        <f t="shared" ref="L40" ca="1" si="139">RANDBETWEEN(20,60)+L39</f>
+        <v>538</v>
       </c>
       <c r="M40" s="105">
-        <f t="shared" ref="M40" ca="1" si="149">RANDBETWEEN(20,60)+M39</f>
-        <v>521</v>
+        <f t="shared" ref="M40" ca="1" si="140">RANDBETWEEN(20,60)+M39</f>
+        <v>558</v>
       </c>
       <c r="N40" s="105">
-        <f t="shared" ref="N40" ca="1" si="150">RANDBETWEEN(20,60)+N39</f>
-        <v>541</v>
+        <f t="shared" ref="N40" ca="1" si="141">RANDBETWEEN(20,60)+N39</f>
+        <v>529</v>
       </c>
       <c r="O40" s="105">
-        <f t="shared" ref="O40" ca="1" si="151">RANDBETWEEN(20,60)+O39</f>
-        <v>529</v>
+        <f t="shared" ref="O40" ca="1" si="142">RANDBETWEEN(20,60)+O39</f>
+        <v>525</v>
       </c>
       <c r="P40" s="105">
-        <f t="shared" ref="P40" ca="1" si="152">RANDBETWEEN(20,60)+P39</f>
-        <v>557</v>
+        <f t="shared" ref="P40" ca="1" si="143">RANDBETWEEN(20,60)+P39</f>
+        <v>550</v>
       </c>
       <c r="Q40" s="105">
-        <f t="shared" ref="Q40" ca="1" si="153">RANDBETWEEN(20,60)+Q39</f>
-        <v>525</v>
-      </c>
-      <c r="R40" s="105">
-        <f t="shared" ref="R40" ca="1" si="154">RANDBETWEEN(20,60)+R39</f>
-        <v>523</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" ref="Q40" ca="1" si="144">RANDBETWEEN(20,60)+Q39</f>
+        <v>527</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="123" t="s">
         <v>32</v>
       </c>
@@ -23284,67 +23141,63 @@
         <v>53</v>
       </c>
       <c r="D41" s="105">
-        <f t="shared" ref="D41:R41" ca="1" si="155">D40-D39</f>
-        <v>43</v>
+        <f t="shared" ref="D41:Q41" ca="1" si="145">D40-D39</f>
+        <v>42</v>
       </c>
       <c r="E41" s="105">
-        <f t="shared" ca="1" si="155"/>
-        <v>56</v>
+        <f t="shared" ca="1" si="145"/>
+        <v>30</v>
       </c>
       <c r="F41" s="105">
-        <f t="shared" ca="1" si="155"/>
-        <v>32</v>
+        <f t="shared" ca="1" si="145"/>
+        <v>23</v>
       </c>
       <c r="G41" s="105">
-        <f t="shared" ca="1" si="155"/>
+        <f t="shared" ca="1" si="145"/>
         <v>55</v>
       </c>
       <c r="H41" s="105">
-        <f t="shared" ca="1" si="155"/>
-        <v>33</v>
+        <f t="shared" ca="1" si="145"/>
+        <v>48</v>
       </c>
       <c r="I41" s="105">
-        <f t="shared" ca="1" si="155"/>
-        <v>57</v>
+        <f t="shared" ca="1" si="145"/>
+        <v>49</v>
       </c>
       <c r="J41" s="105">
-        <f t="shared" ca="1" si="155"/>
-        <v>33</v>
+        <f t="shared" ca="1" si="145"/>
+        <v>48</v>
       </c>
       <c r="K41" s="105">
-        <f t="shared" ca="1" si="155"/>
-        <v>47</v>
+        <f t="shared" ca="1" si="145"/>
+        <v>36</v>
       </c>
       <c r="L41" s="105">
-        <f t="shared" ca="1" si="155"/>
-        <v>43</v>
+        <f t="shared" ca="1" si="145"/>
+        <v>38</v>
       </c>
       <c r="M41" s="105">
-        <f t="shared" ca="1" si="155"/>
-        <v>21</v>
+        <f t="shared" ca="1" si="145"/>
+        <v>58</v>
       </c>
       <c r="N41" s="105">
-        <f t="shared" ca="1" si="155"/>
-        <v>41</v>
+        <f t="shared" ca="1" si="145"/>
+        <v>29</v>
       </c>
       <c r="O41" s="105">
-        <f t="shared" ca="1" si="155"/>
-        <v>29</v>
+        <f t="shared" ca="1" si="145"/>
+        <v>25</v>
       </c>
       <c r="P41" s="105">
-        <f t="shared" ca="1" si="155"/>
-        <v>57</v>
+        <f t="shared" ca="1" si="145"/>
+        <v>50</v>
       </c>
       <c r="Q41" s="105">
-        <f t="shared" ca="1" si="155"/>
-        <v>25</v>
-      </c>
-      <c r="R41" s="105">
-        <f t="shared" ca="1" si="155"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="145"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="123" t="s">
         <v>32</v>
       </c>
@@ -23396,11 +23249,8 @@
       <c r="Q42" s="105">
         <v>500</v>
       </c>
-      <c r="R42" s="105">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="123" t="s">
         <v>32</v>
       </c>
@@ -23412,66 +23262,62 @@
       </c>
       <c r="D43" s="105">
         <f ca="1">RANDBETWEEN(20,60)+D42</f>
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="E43" s="105">
-        <f t="shared" ref="E43" ca="1" si="156">RANDBETWEEN(20,60)+E42</f>
-        <v>539</v>
+        <f t="shared" ref="E43" ca="1" si="146">RANDBETWEEN(20,60)+E42</f>
+        <v>522</v>
       </c>
       <c r="F43" s="105">
-        <f t="shared" ref="F43" ca="1" si="157">RANDBETWEEN(20,60)+F42</f>
-        <v>545</v>
+        <f t="shared" ref="F43" ca="1" si="147">RANDBETWEEN(20,60)+F42</f>
+        <v>535</v>
       </c>
       <c r="G43" s="105">
-        <f t="shared" ref="G43" ca="1" si="158">RANDBETWEEN(20,60)+G42</f>
-        <v>535</v>
+        <f t="shared" ref="G43" ca="1" si="148">RANDBETWEEN(20,60)+G42</f>
+        <v>548</v>
       </c>
       <c r="H43" s="105">
-        <f t="shared" ref="H43" ca="1" si="159">RANDBETWEEN(20,60)+H42</f>
+        <f t="shared" ref="H43" ca="1" si="149">RANDBETWEEN(20,60)+H42</f>
+        <v>530</v>
+      </c>
+      <c r="I43" s="105">
+        <f t="shared" ref="I43" ca="1" si="150">RANDBETWEEN(20,60)+I42</f>
+        <v>524</v>
+      </c>
+      <c r="J43" s="105">
+        <f t="shared" ref="J43" ca="1" si="151">RANDBETWEEN(20,60)+J42</f>
         <v>538</v>
       </c>
-      <c r="I43" s="105">
-        <f t="shared" ref="I43" ca="1" si="160">RANDBETWEEN(20,60)+I42</f>
-        <v>559</v>
-      </c>
-      <c r="J43" s="105">
-        <f t="shared" ref="J43" ca="1" si="161">RANDBETWEEN(20,60)+J42</f>
-        <v>545</v>
-      </c>
       <c r="K43" s="105">
-        <f t="shared" ref="K43" ca="1" si="162">RANDBETWEEN(20,60)+K42</f>
-        <v>530</v>
+        <f t="shared" ref="K43" ca="1" si="152">RANDBETWEEN(20,60)+K42</f>
+        <v>524</v>
       </c>
       <c r="L43" s="105">
-        <f t="shared" ref="L43" ca="1" si="163">RANDBETWEEN(20,60)+L42</f>
-        <v>529</v>
+        <f t="shared" ref="L43" ca="1" si="153">RANDBETWEEN(20,60)+L42</f>
+        <v>558</v>
       </c>
       <c r="M43" s="105">
-        <f t="shared" ref="M43" ca="1" si="164">RANDBETWEEN(20,60)+M42</f>
-        <v>542</v>
+        <f t="shared" ref="M43" ca="1" si="154">RANDBETWEEN(20,60)+M42</f>
+        <v>551</v>
       </c>
       <c r="N43" s="105">
-        <f t="shared" ref="N43" ca="1" si="165">RANDBETWEEN(20,60)+N42</f>
-        <v>520</v>
+        <f t="shared" ref="N43" ca="1" si="155">RANDBETWEEN(20,60)+N42</f>
+        <v>540</v>
       </c>
       <c r="O43" s="105">
-        <f t="shared" ref="O43" ca="1" si="166">RANDBETWEEN(20,60)+O42</f>
-        <v>552</v>
+        <f t="shared" ref="O43" ca="1" si="156">RANDBETWEEN(20,60)+O42</f>
+        <v>548</v>
       </c>
       <c r="P43" s="105">
-        <f t="shared" ref="P43" ca="1" si="167">RANDBETWEEN(20,60)+P42</f>
-        <v>535</v>
+        <f t="shared" ref="P43" ca="1" si="157">RANDBETWEEN(20,60)+P42</f>
+        <v>560</v>
       </c>
       <c r="Q43" s="105">
-        <f t="shared" ref="Q43" ca="1" si="168">RANDBETWEEN(20,60)+Q42</f>
-        <v>527</v>
-      </c>
-      <c r="R43" s="105">
-        <f t="shared" ref="R43" ca="1" si="169">RANDBETWEEN(20,60)+R42</f>
-        <v>539</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" ref="Q43" ca="1" si="158">RANDBETWEEN(20,60)+Q42</f>
+        <v>547</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="123" t="s">
         <v>32</v>
       </c>
@@ -23482,67 +23328,63 @@
         <v>53</v>
       </c>
       <c r="D44" s="105">
-        <f t="shared" ref="D44:R44" ca="1" si="170">D43-D42</f>
-        <v>26</v>
+        <f t="shared" ref="D44:Q44" ca="1" si="159">D43-D42</f>
+        <v>20</v>
       </c>
       <c r="E44" s="105">
-        <f t="shared" ca="1" si="170"/>
-        <v>39</v>
+        <f t="shared" ca="1" si="159"/>
+        <v>22</v>
       </c>
       <c r="F44" s="105">
-        <f t="shared" ca="1" si="170"/>
-        <v>45</v>
+        <f t="shared" ca="1" si="159"/>
+        <v>35</v>
       </c>
       <c r="G44" s="105">
-        <f t="shared" ca="1" si="170"/>
-        <v>35</v>
+        <f t="shared" ca="1" si="159"/>
+        <v>48</v>
       </c>
       <c r="H44" s="105">
-        <f t="shared" ca="1" si="170"/>
+        <f t="shared" ca="1" si="159"/>
+        <v>30</v>
+      </c>
+      <c r="I44" s="105">
+        <f t="shared" ca="1" si="159"/>
+        <v>24</v>
+      </c>
+      <c r="J44" s="105">
+        <f t="shared" ca="1" si="159"/>
         <v>38</v>
       </c>
-      <c r="I44" s="105">
-        <f t="shared" ca="1" si="170"/>
-        <v>59</v>
-      </c>
-      <c r="J44" s="105">
-        <f t="shared" ca="1" si="170"/>
-        <v>45</v>
-      </c>
       <c r="K44" s="105">
-        <f t="shared" ca="1" si="170"/>
-        <v>30</v>
+        <f t="shared" ca="1" si="159"/>
+        <v>24</v>
       </c>
       <c r="L44" s="105">
-        <f t="shared" ca="1" si="170"/>
-        <v>29</v>
+        <f t="shared" ca="1" si="159"/>
+        <v>58</v>
       </c>
       <c r="M44" s="105">
-        <f t="shared" ca="1" si="170"/>
-        <v>42</v>
+        <f t="shared" ca="1" si="159"/>
+        <v>51</v>
       </c>
       <c r="N44" s="105">
-        <f t="shared" ca="1" si="170"/>
-        <v>20</v>
+        <f t="shared" ca="1" si="159"/>
+        <v>40</v>
       </c>
       <c r="O44" s="105">
-        <f t="shared" ca="1" si="170"/>
-        <v>52</v>
+        <f t="shared" ca="1" si="159"/>
+        <v>48</v>
       </c>
       <c r="P44" s="105">
-        <f t="shared" ca="1" si="170"/>
-        <v>35</v>
+        <f t="shared" ca="1" si="159"/>
+        <v>60</v>
       </c>
       <c r="Q44" s="105">
-        <f t="shared" ca="1" si="170"/>
-        <v>27</v>
-      </c>
-      <c r="R44" s="105">
-        <f t="shared" ca="1" si="170"/>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="159"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="123" t="s">
         <v>32</v>
       </c>
@@ -23594,11 +23436,8 @@
       <c r="Q45" s="105">
         <v>500</v>
       </c>
-      <c r="R45" s="105">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="123" t="s">
         <v>32</v>
       </c>
@@ -23610,66 +23449,62 @@
       </c>
       <c r="D46" s="105">
         <f ca="1">RANDBETWEEN(20,60)+D45</f>
-        <v>547</v>
+        <v>558</v>
       </c>
       <c r="E46" s="105">
-        <f t="shared" ref="E46" ca="1" si="171">RANDBETWEEN(20,60)+E45</f>
+        <f t="shared" ref="E46" ca="1" si="160">RANDBETWEEN(20,60)+E45</f>
+        <v>529</v>
+      </c>
+      <c r="F46" s="105">
+        <f t="shared" ref="F46" ca="1" si="161">RANDBETWEEN(20,60)+F45</f>
+        <v>551</v>
+      </c>
+      <c r="G46" s="105">
+        <f t="shared" ref="G46" ca="1" si="162">RANDBETWEEN(20,60)+G45</f>
+        <v>539</v>
+      </c>
+      <c r="H46" s="105">
+        <f t="shared" ref="H46" ca="1" si="163">RANDBETWEEN(20,60)+H45</f>
+        <v>539</v>
+      </c>
+      <c r="I46" s="105">
+        <f t="shared" ref="I46" ca="1" si="164">RANDBETWEEN(20,60)+I45</f>
+        <v>542</v>
+      </c>
+      <c r="J46" s="105">
+        <f t="shared" ref="J46" ca="1" si="165">RANDBETWEEN(20,60)+J45</f>
+        <v>553</v>
+      </c>
+      <c r="K46" s="105">
+        <f t="shared" ref="K46" ca="1" si="166">RANDBETWEEN(20,60)+K45</f>
+        <v>524</v>
+      </c>
+      <c r="L46" s="105">
+        <f t="shared" ref="L46" ca="1" si="167">RANDBETWEEN(20,60)+L45</f>
+        <v>539</v>
+      </c>
+      <c r="M46" s="105">
+        <f t="shared" ref="M46" ca="1" si="168">RANDBETWEEN(20,60)+M45</f>
+        <v>545</v>
+      </c>
+      <c r="N46" s="105">
+        <f t="shared" ref="N46" ca="1" si="169">RANDBETWEEN(20,60)+N45</f>
+        <v>527</v>
+      </c>
+      <c r="O46" s="105">
+        <f t="shared" ref="O46" ca="1" si="170">RANDBETWEEN(20,60)+O45</f>
         <v>521</v>
       </c>
-      <c r="F46" s="105">
-        <f t="shared" ref="F46" ca="1" si="172">RANDBETWEEN(20,60)+F45</f>
+      <c r="P46" s="105">
+        <f t="shared" ref="P46" ca="1" si="171">RANDBETWEEN(20,60)+P45</f>
+        <v>541</v>
+      </c>
+      <c r="Q46" s="105">
+        <f t="shared" ref="Q46" ca="1" si="172">RANDBETWEEN(20,60)+Q45</f>
         <v>529</v>
       </c>
-      <c r="G46" s="105">
-        <f t="shared" ref="G46" ca="1" si="173">RANDBETWEEN(20,60)+G45</f>
-        <v>526</v>
-      </c>
-      <c r="H46" s="105">
-        <f t="shared" ref="H46" ca="1" si="174">RANDBETWEEN(20,60)+H45</f>
-        <v>545</v>
-      </c>
-      <c r="I46" s="105">
-        <f t="shared" ref="I46" ca="1" si="175">RANDBETWEEN(20,60)+I45</f>
-        <v>531</v>
-      </c>
-      <c r="J46" s="105">
-        <f t="shared" ref="J46" ca="1" si="176">RANDBETWEEN(20,60)+J45</f>
-        <v>553</v>
-      </c>
-      <c r="K46" s="105">
-        <f t="shared" ref="K46" ca="1" si="177">RANDBETWEEN(20,60)+K45</f>
-        <v>521</v>
-      </c>
-      <c r="L46" s="105">
-        <f t="shared" ref="L46" ca="1" si="178">RANDBETWEEN(20,60)+L45</f>
-        <v>544</v>
-      </c>
-      <c r="M46" s="105">
-        <f t="shared" ref="M46" ca="1" si="179">RANDBETWEEN(20,60)+M45</f>
-        <v>526</v>
-      </c>
-      <c r="N46" s="105">
-        <f t="shared" ref="N46" ca="1" si="180">RANDBETWEEN(20,60)+N45</f>
-        <v>535</v>
-      </c>
-      <c r="O46" s="105">
-        <f t="shared" ref="O46" ca="1" si="181">RANDBETWEEN(20,60)+O45</f>
-        <v>542</v>
-      </c>
-      <c r="P46" s="105">
-        <f t="shared" ref="P46" ca="1" si="182">RANDBETWEEN(20,60)+P45</f>
-        <v>532</v>
-      </c>
-      <c r="Q46" s="105">
-        <f t="shared" ref="Q46" ca="1" si="183">RANDBETWEEN(20,60)+Q45</f>
-        <v>526</v>
-      </c>
-      <c r="R46" s="105">
-        <f t="shared" ref="R46" ca="1" si="184">RANDBETWEEN(20,60)+R45</f>
-        <v>555</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="123" t="s">
         <v>32</v>
       </c>
@@ -23680,71 +23515,67 @@
         <v>53</v>
       </c>
       <c r="D47" s="105">
-        <f t="shared" ref="D47:R47" ca="1" si="185">D46-D45</f>
-        <v>47</v>
+        <f t="shared" ref="D47:Q47" ca="1" si="173">D46-D45</f>
+        <v>58</v>
       </c>
       <c r="E47" s="105">
-        <f t="shared" ca="1" si="185"/>
+        <f t="shared" ca="1" si="173"/>
+        <v>29</v>
+      </c>
+      <c r="F47" s="105">
+        <f t="shared" ca="1" si="173"/>
+        <v>51</v>
+      </c>
+      <c r="G47" s="105">
+        <f t="shared" ca="1" si="173"/>
+        <v>39</v>
+      </c>
+      <c r="H47" s="105">
+        <f t="shared" ca="1" si="173"/>
+        <v>39</v>
+      </c>
+      <c r="I47" s="105">
+        <f t="shared" ca="1" si="173"/>
+        <v>42</v>
+      </c>
+      <c r="J47" s="105">
+        <f t="shared" ca="1" si="173"/>
+        <v>53</v>
+      </c>
+      <c r="K47" s="105">
+        <f t="shared" ca="1" si="173"/>
+        <v>24</v>
+      </c>
+      <c r="L47" s="105">
+        <f t="shared" ca="1" si="173"/>
+        <v>39</v>
+      </c>
+      <c r="M47" s="105">
+        <f t="shared" ca="1" si="173"/>
+        <v>45</v>
+      </c>
+      <c r="N47" s="105">
+        <f t="shared" ca="1" si="173"/>
+        <v>27</v>
+      </c>
+      <c r="O47" s="105">
+        <f t="shared" ca="1" si="173"/>
         <v>21</v>
       </c>
-      <c r="F47" s="105">
-        <f t="shared" ca="1" si="185"/>
+      <c r="P47" s="105">
+        <f t="shared" ca="1" si="173"/>
+        <v>41</v>
+      </c>
+      <c r="Q47" s="105">
+        <f t="shared" ca="1" si="173"/>
         <v>29</v>
-      </c>
-      <c r="G47" s="105">
-        <f t="shared" ca="1" si="185"/>
-        <v>26</v>
-      </c>
-      <c r="H47" s="105">
-        <f t="shared" ca="1" si="185"/>
-        <v>45</v>
-      </c>
-      <c r="I47" s="105">
-        <f t="shared" ca="1" si="185"/>
-        <v>31</v>
-      </c>
-      <c r="J47" s="105">
-        <f t="shared" ca="1" si="185"/>
-        <v>53</v>
-      </c>
-      <c r="K47" s="105">
-        <f t="shared" ca="1" si="185"/>
-        <v>21</v>
-      </c>
-      <c r="L47" s="105">
-        <f t="shared" ca="1" si="185"/>
-        <v>44</v>
-      </c>
-      <c r="M47" s="105">
-        <f t="shared" ca="1" si="185"/>
-        <v>26</v>
-      </c>
-      <c r="N47" s="105">
-        <f t="shared" ca="1" si="185"/>
-        <v>35</v>
-      </c>
-      <c r="O47" s="105">
-        <f t="shared" ca="1" si="185"/>
-        <v>42</v>
-      </c>
-      <c r="P47" s="105">
-        <f t="shared" ca="1" si="185"/>
-        <v>32</v>
-      </c>
-      <c r="Q47" s="105">
-        <f t="shared" ca="1" si="185"/>
-        <v>26</v>
-      </c>
-      <c r="R47" s="105">
-        <f t="shared" ca="1" si="185"/>
-        <v>55</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
-    <mergeCell ref="D1:R1"/>
+    <mergeCell ref="D1:Q1"/>
     <mergeCell ref="A3:A17"/>
     <mergeCell ref="A18:A32"/>
     <mergeCell ref="A33:A47"/>
@@ -23771,8 +23602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q46" sqref="Q46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23793,46 +23624,46 @@
         <v>39</v>
       </c>
       <c r="D1" s="120">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E1" s="120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F1" s="120">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G1" s="120">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H1" s="120">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I1" s="120">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J1" s="120">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K1" s="120">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L1" s="120">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M1" s="120">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N1" s="120">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O1" s="120">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P1" s="120">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q1" s="120">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="R1" s="120"/>
     </row>

</xml_diff>

<commit_message>
adjust spreadsheet for spores/no spores
</commit_message>
<xml_diff>
--- a/inst/Example/Mouse_Experiment_Example.xlsx
+++ b/inst/Example/Mouse_Experiment_Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtcoll06\Box\Lab Docs\R projects\mouseR\inst\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E156B40-5ED5-4E4F-8F0E-3119265A0E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B4B37F-EFC6-44C0-8C36-A6CC0EA51260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20689,8 +20689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="R2" sqref="R1:R1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q47" sqref="Q47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20831,51 +20831,51 @@
       </c>
       <c r="D4" s="103">
         <f ca="1">RANDBETWEEN(20,60)+D3</f>
-        <v>552</v>
+        <v>520</v>
       </c>
       <c r="E4" s="119">
         <f t="shared" ref="E4:Q4" ca="1" si="0">RANDBETWEEN(20,60)+E3</f>
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="F4" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>522</v>
+        <v>539</v>
       </c>
       <c r="G4" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="H4" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>545</v>
+        <v>552</v>
       </c>
       <c r="I4" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>558</v>
+        <v>549</v>
       </c>
       <c r="J4" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>551</v>
+        <v>537</v>
       </c>
       <c r="K4" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>551</v>
+        <v>536</v>
       </c>
       <c r="L4" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="M4" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>526</v>
+        <v>546</v>
       </c>
       <c r="N4" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>550</v>
+        <v>525</v>
       </c>
       <c r="O4" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>525</v>
+        <v>559</v>
       </c>
       <c r="P4" s="119">
         <f t="shared" ca="1" si="0"/>
@@ -20883,7 +20883,7 @@
       </c>
       <c r="Q4" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>558</v>
+        <v>545</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -20898,51 +20898,51 @@
       </c>
       <c r="D5" s="103">
         <f t="shared" ref="D5:Q5" ca="1" si="1">D4-D3</f>
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="E5" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F5" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="G5" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H5" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="I5" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="J5" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="K5" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="L5" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="M5" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="N5" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="O5" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="P5" s="103">
         <f t="shared" ca="1" si="1"/>
@@ -20950,7 +20950,7 @@
       </c>
       <c r="Q5" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -21018,59 +21018,59 @@
       </c>
       <c r="D7" s="119">
         <f ca="1">RANDBETWEEN(20,60)+D6</f>
-        <v>549</v>
+        <v>525</v>
       </c>
       <c r="E7" s="119">
         <f t="shared" ref="E7:Q7" ca="1" si="2">RANDBETWEEN(20,60)+E6</f>
-        <v>542</v>
+        <v>558</v>
       </c>
       <c r="F7" s="119">
         <f t="shared" ca="1" si="2"/>
-        <v>536</v>
+        <v>546</v>
       </c>
       <c r="G7" s="119">
         <f t="shared" ca="1" si="2"/>
-        <v>554</v>
+        <v>521</v>
       </c>
       <c r="H7" s="119">
         <f t="shared" ca="1" si="2"/>
-        <v>554</v>
+        <v>524</v>
       </c>
       <c r="I7" s="119">
         <f t="shared" ca="1" si="2"/>
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="J7" s="119">
         <f t="shared" ca="1" si="2"/>
-        <v>547</v>
+        <v>556</v>
       </c>
       <c r="K7" s="119">
         <f t="shared" ca="1" si="2"/>
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="L7" s="119">
         <f t="shared" ca="1" si="2"/>
-        <v>537</v>
+        <v>528</v>
       </c>
       <c r="M7" s="119">
         <f t="shared" ca="1" si="2"/>
-        <v>520</v>
+        <v>538</v>
       </c>
       <c r="N7" s="119">
         <f t="shared" ca="1" si="2"/>
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="O7" s="119">
         <f t="shared" ca="1" si="2"/>
-        <v>540</v>
+        <v>552</v>
       </c>
       <c r="P7" s="119">
         <f t="shared" ca="1" si="2"/>
-        <v>553</v>
+        <v>528</v>
       </c>
       <c r="Q7" s="119">
         <f t="shared" ca="1" si="2"/>
-        <v>539</v>
+        <v>526</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -21085,59 +21085,59 @@
       </c>
       <c r="D8" s="103">
         <f t="shared" ref="D8:Q8" ca="1" si="3">D7-D6</f>
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="E8" s="103">
         <f t="shared" ca="1" si="3"/>
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="F8" s="103">
         <f t="shared" ca="1" si="3"/>
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="G8" s="103">
         <f t="shared" ca="1" si="3"/>
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="H8" s="103">
         <f t="shared" ca="1" si="3"/>
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="I8" s="103">
         <f t="shared" ca="1" si="3"/>
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="J8" s="103">
         <f t="shared" ca="1" si="3"/>
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="K8" s="103">
         <f t="shared" ca="1" si="3"/>
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L8" s="103">
         <f t="shared" ca="1" si="3"/>
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="M8" s="103">
         <f t="shared" ca="1" si="3"/>
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="N8" s="103">
         <f t="shared" ca="1" si="3"/>
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="O8" s="103">
         <f t="shared" ca="1" si="3"/>
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="P8" s="103">
         <f t="shared" ca="1" si="3"/>
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="Q8" s="103">
         <f t="shared" ca="1" si="3"/>
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -21205,59 +21205,59 @@
       </c>
       <c r="D10" s="103">
         <f ca="1">RANDBETWEEN(20,60)+D9</f>
-        <v>550</v>
+        <v>537</v>
       </c>
       <c r="E10" s="119">
         <f t="shared" ref="E10:Q10" ca="1" si="4">RANDBETWEEN(20,60)+E9</f>
-        <v>546</v>
+        <v>539</v>
       </c>
       <c r="F10" s="119">
         <f t="shared" ca="1" si="4"/>
-        <v>527</v>
+        <v>536</v>
       </c>
       <c r="G10" s="119">
         <f t="shared" ca="1" si="4"/>
-        <v>523</v>
+        <v>541</v>
       </c>
       <c r="H10" s="119">
         <f t="shared" ca="1" si="4"/>
-        <v>551</v>
+        <v>528</v>
       </c>
       <c r="I10" s="119">
         <f t="shared" ca="1" si="4"/>
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J10" s="119">
         <f t="shared" ca="1" si="4"/>
-        <v>540</v>
+        <v>532</v>
       </c>
       <c r="K10" s="119">
         <f t="shared" ca="1" si="4"/>
-        <v>533</v>
+        <v>555</v>
       </c>
       <c r="L10" s="119">
         <f t="shared" ca="1" si="4"/>
-        <v>537</v>
+        <v>553</v>
       </c>
       <c r="M10" s="119">
         <f t="shared" ca="1" si="4"/>
-        <v>542</v>
+        <v>551</v>
       </c>
       <c r="N10" s="119">
         <f t="shared" ca="1" si="4"/>
-        <v>546</v>
+        <v>533</v>
       </c>
       <c r="O10" s="119">
         <f t="shared" ca="1" si="4"/>
-        <v>556</v>
+        <v>523</v>
       </c>
       <c r="P10" s="119">
         <f t="shared" ca="1" si="4"/>
-        <v>520</v>
+        <v>538</v>
       </c>
       <c r="Q10" s="119">
         <f t="shared" ca="1" si="4"/>
-        <v>558</v>
+        <v>527</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -21272,59 +21272,59 @@
       </c>
       <c r="D11" s="103">
         <f t="shared" ref="D11:Q11" ca="1" si="5">D10-D9</f>
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="E11" s="103">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F11" s="103">
         <f t="shared" ca="1" si="5"/>
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="G11" s="103">
         <f t="shared" ca="1" si="5"/>
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="H11" s="103">
         <f t="shared" ca="1" si="5"/>
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="I11" s="103">
         <f t="shared" ca="1" si="5"/>
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="J11" s="103">
         <f t="shared" ca="1" si="5"/>
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="K11" s="103">
         <f t="shared" ca="1" si="5"/>
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="L11" s="103">
         <f t="shared" ca="1" si="5"/>
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="M11" s="103">
         <f t="shared" ca="1" si="5"/>
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="N11" s="103">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="O11" s="103">
         <f t="shared" ca="1" si="5"/>
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="P11" s="103">
         <f t="shared" ca="1" si="5"/>
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="Q11" s="103">
         <f t="shared" ca="1" si="5"/>
-        <v>58</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -21392,59 +21392,59 @@
       </c>
       <c r="D13" s="119">
         <f ca="1">RANDBETWEEN(20,60)+D12</f>
-        <v>550</v>
+        <v>521</v>
       </c>
       <c r="E13" s="119">
         <f t="shared" ref="E13" ca="1" si="6">RANDBETWEEN(20,60)+E12</f>
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="F13" s="119">
         <f t="shared" ref="F13" ca="1" si="7">RANDBETWEEN(20,60)+F12</f>
-        <v>546</v>
+        <v>527</v>
       </c>
       <c r="G13" s="119">
         <f t="shared" ref="G13" ca="1" si="8">RANDBETWEEN(20,60)+G12</f>
-        <v>546</v>
+        <v>539</v>
       </c>
       <c r="H13" s="119">
         <f t="shared" ref="H13" ca="1" si="9">RANDBETWEEN(20,60)+H12</f>
-        <v>549</v>
+        <v>533</v>
       </c>
       <c r="I13" s="119">
         <f t="shared" ref="I13" ca="1" si="10">RANDBETWEEN(20,60)+I12</f>
-        <v>525</v>
+        <v>537</v>
       </c>
       <c r="J13" s="119">
         <f t="shared" ref="J13" ca="1" si="11">RANDBETWEEN(20,60)+J12</f>
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="K13" s="119">
         <f t="shared" ref="K13" ca="1" si="12">RANDBETWEEN(20,60)+K12</f>
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="L13" s="119">
         <f t="shared" ref="L13" ca="1" si="13">RANDBETWEEN(20,60)+L12</f>
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="M13" s="119">
         <f t="shared" ref="M13" ca="1" si="14">RANDBETWEEN(20,60)+M12</f>
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="N13" s="119">
         <f t="shared" ref="N13" ca="1" si="15">RANDBETWEEN(20,60)+N12</f>
-        <v>546</v>
+        <v>528</v>
       </c>
       <c r="O13" s="119">
         <f t="shared" ref="O13" ca="1" si="16">RANDBETWEEN(20,60)+O12</f>
-        <v>537</v>
+        <v>527</v>
       </c>
       <c r="P13" s="119">
         <f t="shared" ref="P13" ca="1" si="17">RANDBETWEEN(20,60)+P12</f>
-        <v>538</v>
+        <v>558</v>
       </c>
       <c r="Q13" s="119">
         <f t="shared" ref="Q13" ca="1" si="18">RANDBETWEEN(20,60)+Q12</f>
-        <v>524</v>
+        <v>558</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -21459,59 +21459,59 @@
       </c>
       <c r="D14" s="103">
         <f t="shared" ref="D14:Q14" ca="1" si="19">D13-D12</f>
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="E14" s="103">
         <f t="shared" ca="1" si="19"/>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F14" s="103">
         <f t="shared" ca="1" si="19"/>
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="G14" s="103">
         <f t="shared" ca="1" si="19"/>
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="H14" s="103">
         <f t="shared" ca="1" si="19"/>
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="I14" s="103">
         <f t="shared" ca="1" si="19"/>
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="J14" s="103">
         <f t="shared" ca="1" si="19"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K14" s="103">
         <f t="shared" ca="1" si="19"/>
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="L14" s="103">
         <f t="shared" ca="1" si="19"/>
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M14" s="103">
         <f t="shared" ca="1" si="19"/>
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="N14" s="103">
         <f t="shared" ca="1" si="19"/>
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="O14" s="103">
         <f t="shared" ca="1" si="19"/>
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="P14" s="103">
         <f t="shared" ca="1" si="19"/>
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="Q14" s="103">
         <f t="shared" ca="1" si="19"/>
-        <v>24</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -21579,7 +21579,7 @@
       </c>
       <c r="D16" s="119">
         <f ca="1">RANDBETWEEN(20,60)+D15</f>
-        <v>558</v>
+        <v>549</v>
       </c>
       <c r="E16" s="119">
         <f t="shared" ref="E16" ca="1" si="20">RANDBETWEEN(20,60)+E15</f>
@@ -21587,51 +21587,51 @@
       </c>
       <c r="F16" s="119">
         <f t="shared" ref="F16" ca="1" si="21">RANDBETWEEN(20,60)+F15</f>
-        <v>524</v>
+        <v>537</v>
       </c>
       <c r="G16" s="119">
         <f t="shared" ref="G16" ca="1" si="22">RANDBETWEEN(20,60)+G15</f>
-        <v>541</v>
+        <v>547</v>
       </c>
       <c r="H16" s="119">
         <f t="shared" ref="H16" ca="1" si="23">RANDBETWEEN(20,60)+H15</f>
-        <v>537</v>
+        <v>526</v>
       </c>
       <c r="I16" s="119">
         <f t="shared" ref="I16" ca="1" si="24">RANDBETWEEN(20,60)+I15</f>
-        <v>521</v>
+        <v>530</v>
       </c>
       <c r="J16" s="119">
         <f t="shared" ref="J16" ca="1" si="25">RANDBETWEEN(20,60)+J15</f>
-        <v>558</v>
+        <v>546</v>
       </c>
       <c r="K16" s="119">
         <f t="shared" ref="K16" ca="1" si="26">RANDBETWEEN(20,60)+K15</f>
-        <v>533</v>
+        <v>552</v>
       </c>
       <c r="L16" s="119">
         <f t="shared" ref="L16" ca="1" si="27">RANDBETWEEN(20,60)+L15</f>
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="M16" s="119">
         <f t="shared" ref="M16" ca="1" si="28">RANDBETWEEN(20,60)+M15</f>
-        <v>540</v>
+        <v>526</v>
       </c>
       <c r="N16" s="119">
         <f t="shared" ref="N16" ca="1" si="29">RANDBETWEEN(20,60)+N15</f>
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="O16" s="119">
         <f t="shared" ref="O16" ca="1" si="30">RANDBETWEEN(20,60)+O15</f>
-        <v>549</v>
+        <v>522</v>
       </c>
       <c r="P16" s="119">
         <f t="shared" ref="P16" ca="1" si="31">RANDBETWEEN(20,60)+P15</f>
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="Q16" s="119">
         <f t="shared" ref="Q16" ca="1" si="32">RANDBETWEEN(20,60)+Q15</f>
-        <v>559</v>
+        <v>539</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -21646,7 +21646,7 @@
       </c>
       <c r="D17" s="103">
         <f t="shared" ref="D17:Q17" ca="1" si="33">D16-D15</f>
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E17" s="103">
         <f t="shared" ca="1" si="33"/>
@@ -21654,51 +21654,51 @@
       </c>
       <c r="F17" s="103">
         <f t="shared" ca="1" si="33"/>
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="G17" s="103">
         <f t="shared" ca="1" si="33"/>
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="H17" s="103">
         <f t="shared" ca="1" si="33"/>
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="I17" s="103">
         <f t="shared" ca="1" si="33"/>
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="J17" s="103">
         <f t="shared" ca="1" si="33"/>
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="K17" s="103">
         <f t="shared" ca="1" si="33"/>
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="L17" s="103">
         <f t="shared" ca="1" si="33"/>
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="M17" s="103">
         <f t="shared" ca="1" si="33"/>
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="N17" s="103">
         <f t="shared" ca="1" si="33"/>
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="O17" s="103">
         <f t="shared" ca="1" si="33"/>
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="P17" s="103">
         <f t="shared" ca="1" si="33"/>
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="Q17" s="103">
         <f t="shared" ca="1" si="33"/>
-        <v>59</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -21766,59 +21766,59 @@
       </c>
       <c r="D19" s="104">
         <f ca="1">RANDBETWEEN(20,60)+D18</f>
-        <v>542</v>
+        <v>547</v>
       </c>
       <c r="E19" s="104">
         <f t="shared" ref="E19" ca="1" si="34">RANDBETWEEN(20,60)+E18</f>
-        <v>523</v>
+        <v>546</v>
       </c>
       <c r="F19" s="104">
         <f t="shared" ref="F19" ca="1" si="35">RANDBETWEEN(20,60)+F18</f>
-        <v>547</v>
+        <v>530</v>
       </c>
       <c r="G19" s="104">
         <f t="shared" ref="G19" ca="1" si="36">RANDBETWEEN(20,60)+G18</f>
-        <v>544</v>
+        <v>521</v>
       </c>
       <c r="H19" s="104">
         <f t="shared" ref="H19" ca="1" si="37">RANDBETWEEN(20,60)+H18</f>
-        <v>528</v>
+        <v>553</v>
       </c>
       <c r="I19" s="104">
         <f t="shared" ref="I19" ca="1" si="38">RANDBETWEEN(20,60)+I18</f>
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="J19" s="104">
         <f t="shared" ref="J19" ca="1" si="39">RANDBETWEEN(20,60)+J18</f>
-        <v>560</v>
+        <v>544</v>
       </c>
       <c r="K19" s="104">
         <f t="shared" ref="K19" ca="1" si="40">RANDBETWEEN(20,60)+K18</f>
-        <v>556</v>
+        <v>533</v>
       </c>
       <c r="L19" s="104">
         <f t="shared" ref="L19" ca="1" si="41">RANDBETWEEN(20,60)+L18</f>
-        <v>545</v>
+        <v>528</v>
       </c>
       <c r="M19" s="104">
         <f t="shared" ref="M19" ca="1" si="42">RANDBETWEEN(20,60)+M18</f>
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="N19" s="104">
         <f t="shared" ref="N19" ca="1" si="43">RANDBETWEEN(20,60)+N18</f>
-        <v>524</v>
+        <v>538</v>
       </c>
       <c r="O19" s="104">
         <f t="shared" ref="O19" ca="1" si="44">RANDBETWEEN(20,60)+O18</f>
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="P19" s="104">
         <f t="shared" ref="P19" ca="1" si="45">RANDBETWEEN(20,60)+P18</f>
-        <v>531</v>
+        <v>536</v>
       </c>
       <c r="Q19" s="104">
         <f t="shared" ref="Q19" ca="1" si="46">RANDBETWEEN(20,60)+Q18</f>
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -21833,59 +21833,59 @@
       </c>
       <c r="D20" s="104">
         <f t="shared" ref="D20:Q20" ca="1" si="47">D19-D18</f>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E20" s="104">
         <f t="shared" ca="1" si="47"/>
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="F20" s="104">
         <f t="shared" ca="1" si="47"/>
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="G20" s="104">
         <f t="shared" ca="1" si="47"/>
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="H20" s="104">
         <f t="shared" ca="1" si="47"/>
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="I20" s="104">
         <f t="shared" ca="1" si="47"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J20" s="104">
         <f t="shared" ca="1" si="47"/>
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="K20" s="104">
         <f t="shared" ca="1" si="47"/>
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="L20" s="104">
         <f t="shared" ca="1" si="47"/>
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="M20" s="104">
         <f t="shared" ca="1" si="47"/>
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="N20" s="104">
         <f t="shared" ca="1" si="47"/>
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="O20" s="104">
         <f t="shared" ca="1" si="47"/>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P20" s="104">
         <f t="shared" ca="1" si="47"/>
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="Q20" s="104">
         <f t="shared" ca="1" si="47"/>
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -21953,59 +21953,59 @@
       </c>
       <c r="D22" s="104">
         <f ca="1">RANDBETWEEN(20,60)+D21</f>
-        <v>528</v>
+        <v>556</v>
       </c>
       <c r="E22" s="104">
         <f t="shared" ref="E22" ca="1" si="48">RANDBETWEEN(20,60)+E21</f>
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="F22" s="104">
         <f t="shared" ref="F22" ca="1" si="49">RANDBETWEEN(20,60)+F21</f>
-        <v>532</v>
+        <v>549</v>
       </c>
       <c r="G22" s="104">
         <f t="shared" ref="G22" ca="1" si="50">RANDBETWEEN(20,60)+G21</f>
-        <v>545</v>
+        <v>532</v>
       </c>
       <c r="H22" s="104">
         <f t="shared" ref="H22" ca="1" si="51">RANDBETWEEN(20,60)+H21</f>
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="I22" s="104">
         <f t="shared" ref="I22" ca="1" si="52">RANDBETWEEN(20,60)+I21</f>
-        <v>520</v>
+        <v>559</v>
       </c>
       <c r="J22" s="104">
         <f t="shared" ref="J22" ca="1" si="53">RANDBETWEEN(20,60)+J21</f>
-        <v>535</v>
+        <v>521</v>
       </c>
       <c r="K22" s="104">
         <f t="shared" ref="K22" ca="1" si="54">RANDBETWEEN(20,60)+K21</f>
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="L22" s="104">
         <f t="shared" ref="L22" ca="1" si="55">RANDBETWEEN(20,60)+L21</f>
-        <v>539</v>
+        <v>560</v>
       </c>
       <c r="M22" s="104">
         <f t="shared" ref="M22" ca="1" si="56">RANDBETWEEN(20,60)+M21</f>
-        <v>522</v>
+        <v>537</v>
       </c>
       <c r="N22" s="104">
         <f t="shared" ref="N22" ca="1" si="57">RANDBETWEEN(20,60)+N21</f>
-        <v>528</v>
+        <v>535</v>
       </c>
       <c r="O22" s="104">
         <f t="shared" ref="O22" ca="1" si="58">RANDBETWEEN(20,60)+O21</f>
-        <v>523</v>
+        <v>551</v>
       </c>
       <c r="P22" s="104">
         <f t="shared" ref="P22" ca="1" si="59">RANDBETWEEN(20,60)+P21</f>
-        <v>540</v>
+        <v>529</v>
       </c>
       <c r="Q22" s="104">
         <f t="shared" ref="Q22" ca="1" si="60">RANDBETWEEN(20,60)+Q21</f>
-        <v>545</v>
+        <v>534</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -22020,59 +22020,59 @@
       </c>
       <c r="D23" s="104">
         <f t="shared" ref="D23:Q23" ca="1" si="61">D22-D21</f>
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="E23" s="104">
         <f t="shared" ca="1" si="61"/>
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F23" s="104">
         <f t="shared" ca="1" si="61"/>
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="G23" s="104">
         <f t="shared" ca="1" si="61"/>
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="H23" s="104">
         <f t="shared" ca="1" si="61"/>
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="I23" s="104">
         <f t="shared" ca="1" si="61"/>
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="J23" s="104">
         <f t="shared" ca="1" si="61"/>
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="K23" s="104">
         <f t="shared" ca="1" si="61"/>
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="L23" s="104">
         <f t="shared" ca="1" si="61"/>
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="M23" s="104">
         <f t="shared" ca="1" si="61"/>
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="N23" s="104">
         <f t="shared" ca="1" si="61"/>
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="O23" s="104">
         <f t="shared" ca="1" si="61"/>
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="P23" s="104">
         <f t="shared" ca="1" si="61"/>
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="Q23" s="104">
         <f t="shared" ca="1" si="61"/>
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -22140,59 +22140,59 @@
       </c>
       <c r="D25" s="104">
         <f ca="1">RANDBETWEEN(20,60)+D24</f>
-        <v>524</v>
+        <v>549</v>
       </c>
       <c r="E25" s="104">
         <f t="shared" ref="E25" ca="1" si="62">RANDBETWEEN(20,60)+E24</f>
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="F25" s="104">
         <f t="shared" ref="F25" ca="1" si="63">RANDBETWEEN(20,60)+F24</f>
-        <v>553</v>
+        <v>557</v>
       </c>
       <c r="G25" s="104">
         <f t="shared" ref="G25" ca="1" si="64">RANDBETWEEN(20,60)+G24</f>
-        <v>560</v>
+        <v>532</v>
       </c>
       <c r="H25" s="104">
         <f t="shared" ref="H25" ca="1" si="65">RANDBETWEEN(20,60)+H24</f>
-        <v>552</v>
+        <v>537</v>
       </c>
       <c r="I25" s="104">
         <f t="shared" ref="I25" ca="1" si="66">RANDBETWEEN(20,60)+I24</f>
-        <v>526</v>
+        <v>542</v>
       </c>
       <c r="J25" s="104">
         <f t="shared" ref="J25" ca="1" si="67">RANDBETWEEN(20,60)+J24</f>
-        <v>546</v>
+        <v>531</v>
       </c>
       <c r="K25" s="104">
         <f t="shared" ref="K25" ca="1" si="68">RANDBETWEEN(20,60)+K24</f>
-        <v>555</v>
+        <v>546</v>
       </c>
       <c r="L25" s="104">
         <f t="shared" ref="L25" ca="1" si="69">RANDBETWEEN(20,60)+L24</f>
-        <v>549</v>
+        <v>529</v>
       </c>
       <c r="M25" s="104">
         <f t="shared" ref="M25" ca="1" si="70">RANDBETWEEN(20,60)+M24</f>
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="N25" s="104">
         <f t="shared" ref="N25" ca="1" si="71">RANDBETWEEN(20,60)+N24</f>
-        <v>551</v>
+        <v>520</v>
       </c>
       <c r="O25" s="104">
         <f t="shared" ref="O25" ca="1" si="72">RANDBETWEEN(20,60)+O24</f>
-        <v>531</v>
+        <v>537</v>
       </c>
       <c r="P25" s="104">
         <f t="shared" ref="P25" ca="1" si="73">RANDBETWEEN(20,60)+P24</f>
-        <v>556</v>
+        <v>539</v>
       </c>
       <c r="Q25" s="104">
         <f t="shared" ref="Q25" ca="1" si="74">RANDBETWEEN(20,60)+Q24</f>
-        <v>546</v>
+        <v>522</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -22207,59 +22207,59 @@
       </c>
       <c r="D26" s="104">
         <f t="shared" ref="D26:Q26" ca="1" si="75">D25-D24</f>
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="E26" s="104">
         <f t="shared" ca="1" si="75"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F26" s="104">
         <f t="shared" ca="1" si="75"/>
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G26" s="104">
         <f t="shared" ca="1" si="75"/>
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="H26" s="104">
         <f t="shared" ca="1" si="75"/>
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="I26" s="104">
         <f t="shared" ca="1" si="75"/>
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="J26" s="104">
         <f t="shared" ca="1" si="75"/>
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="K26" s="104">
         <f t="shared" ca="1" si="75"/>
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="L26" s="104">
         <f t="shared" ca="1" si="75"/>
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="M26" s="104">
         <f t="shared" ca="1" si="75"/>
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="N26" s="104">
         <f t="shared" ca="1" si="75"/>
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="O26" s="104">
         <f t="shared" ca="1" si="75"/>
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P26" s="104">
         <f t="shared" ca="1" si="75"/>
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="Q26" s="104">
         <f t="shared" ca="1" si="75"/>
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -22327,55 +22327,55 @@
       </c>
       <c r="D28" s="104">
         <f ca="1">RANDBETWEEN(20,60)+D27</f>
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="E28" s="104">
         <f t="shared" ref="E28" ca="1" si="76">RANDBETWEEN(20,60)+E27</f>
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="F28" s="104">
         <f t="shared" ref="F28" ca="1" si="77">RANDBETWEEN(20,60)+F27</f>
-        <v>539</v>
+        <v>528</v>
       </c>
       <c r="G28" s="104">
         <f t="shared" ref="G28" ca="1" si="78">RANDBETWEEN(20,60)+G27</f>
-        <v>528</v>
+        <v>553</v>
       </c>
       <c r="H28" s="104">
         <f t="shared" ref="H28" ca="1" si="79">RANDBETWEEN(20,60)+H27</f>
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I28" s="104">
         <f t="shared" ref="I28" ca="1" si="80">RANDBETWEEN(20,60)+I27</f>
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J28" s="104">
         <f t="shared" ref="J28" ca="1" si="81">RANDBETWEEN(20,60)+J27</f>
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="K28" s="104">
         <f t="shared" ref="K28" ca="1" si="82">RANDBETWEEN(20,60)+K27</f>
-        <v>539</v>
+        <v>548</v>
       </c>
       <c r="L28" s="104">
         <f t="shared" ref="L28" ca="1" si="83">RANDBETWEEN(20,60)+L27</f>
-        <v>553</v>
+        <v>541</v>
       </c>
       <c r="M28" s="104">
         <f t="shared" ref="M28" ca="1" si="84">RANDBETWEEN(20,60)+M27</f>
-        <v>552</v>
+        <v>526</v>
       </c>
       <c r="N28" s="104">
         <f t="shared" ref="N28" ca="1" si="85">RANDBETWEEN(20,60)+N27</f>
-        <v>521</v>
+        <v>551</v>
       </c>
       <c r="O28" s="104">
         <f t="shared" ref="O28" ca="1" si="86">RANDBETWEEN(20,60)+O27</f>
-        <v>547</v>
+        <v>556</v>
       </c>
       <c r="P28" s="104">
         <f t="shared" ref="P28" ca="1" si="87">RANDBETWEEN(20,60)+P27</f>
-        <v>547</v>
+        <v>521</v>
       </c>
       <c r="Q28" s="104">
         <f t="shared" ref="Q28" ca="1" si="88">RANDBETWEEN(20,60)+Q27</f>
@@ -22394,55 +22394,55 @@
       </c>
       <c r="D29" s="104">
         <f t="shared" ref="D29:Q29" ca="1" si="89">D28-D27</f>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E29" s="104">
         <f t="shared" ca="1" si="89"/>
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F29" s="104">
         <f t="shared" ca="1" si="89"/>
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="G29" s="104">
         <f t="shared" ca="1" si="89"/>
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="H29" s="104">
         <f t="shared" ca="1" si="89"/>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I29" s="104">
         <f t="shared" ca="1" si="89"/>
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J29" s="104">
         <f t="shared" ca="1" si="89"/>
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="K29" s="104">
         <f t="shared" ca="1" si="89"/>
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="L29" s="104">
         <f t="shared" ca="1" si="89"/>
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="M29" s="104">
         <f t="shared" ca="1" si="89"/>
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="N29" s="104">
         <f t="shared" ca="1" si="89"/>
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="O29" s="104">
         <f t="shared" ca="1" si="89"/>
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="P29" s="104">
         <f t="shared" ca="1" si="89"/>
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="Q29" s="104">
         <f t="shared" ca="1" si="89"/>
@@ -22514,23 +22514,23 @@
       </c>
       <c r="D31" s="104">
         <f ca="1">RANDBETWEEN(20,60)+D30</f>
-        <v>540</v>
+        <v>551</v>
       </c>
       <c r="E31" s="104">
         <f t="shared" ref="E31" ca="1" si="90">RANDBETWEEN(20,60)+E30</f>
-        <v>541</v>
+        <v>530</v>
       </c>
       <c r="F31" s="104">
         <f t="shared" ref="F31" ca="1" si="91">RANDBETWEEN(20,60)+F30</f>
-        <v>541</v>
+        <v>559</v>
       </c>
       <c r="G31" s="104">
         <f t="shared" ref="G31" ca="1" si="92">RANDBETWEEN(20,60)+G30</f>
-        <v>538</v>
+        <v>543</v>
       </c>
       <c r="H31" s="104">
         <f t="shared" ref="H31" ca="1" si="93">RANDBETWEEN(20,60)+H30</f>
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="I31" s="104">
         <f t="shared" ref="I31" ca="1" si="94">RANDBETWEEN(20,60)+I30</f>
@@ -22538,35 +22538,35 @@
       </c>
       <c r="J31" s="104">
         <f t="shared" ref="J31" ca="1" si="95">RANDBETWEEN(20,60)+J30</f>
-        <v>542</v>
+        <v>522</v>
       </c>
       <c r="K31" s="104">
         <f t="shared" ref="K31" ca="1" si="96">RANDBETWEEN(20,60)+K30</f>
-        <v>534</v>
+        <v>542</v>
       </c>
       <c r="L31" s="104">
         <f t="shared" ref="L31" ca="1" si="97">RANDBETWEEN(20,60)+L30</f>
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="M31" s="104">
         <f t="shared" ref="M31" ca="1" si="98">RANDBETWEEN(20,60)+M30</f>
-        <v>546</v>
+        <v>536</v>
       </c>
       <c r="N31" s="104">
         <f t="shared" ref="N31" ca="1" si="99">RANDBETWEEN(20,60)+N30</f>
-        <v>536</v>
+        <v>521</v>
       </c>
       <c r="O31" s="104">
         <f t="shared" ref="O31" ca="1" si="100">RANDBETWEEN(20,60)+O30</f>
-        <v>538</v>
+        <v>529</v>
       </c>
       <c r="P31" s="104">
         <f t="shared" ref="P31" ca="1" si="101">RANDBETWEEN(20,60)+P30</f>
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="Q31" s="104">
         <f t="shared" ref="Q31" ca="1" si="102">RANDBETWEEN(20,60)+Q30</f>
-        <v>523</v>
+        <v>544</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -22581,23 +22581,23 @@
       </c>
       <c r="D32" s="104">
         <f t="shared" ref="D32:Q32" ca="1" si="103">D31-D30</f>
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="E32" s="104">
         <f t="shared" ca="1" si="103"/>
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="F32" s="104">
         <f t="shared" ca="1" si="103"/>
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="G32" s="104">
         <f t="shared" ca="1" si="103"/>
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="H32" s="104">
         <f t="shared" ca="1" si="103"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I32" s="104">
         <f t="shared" ca="1" si="103"/>
@@ -22605,35 +22605,35 @@
       </c>
       <c r="J32" s="104">
         <f t="shared" ca="1" si="103"/>
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="K32" s="104">
         <f t="shared" ca="1" si="103"/>
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="L32" s="104">
         <f t="shared" ca="1" si="103"/>
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="M32" s="104">
         <f t="shared" ca="1" si="103"/>
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="N32" s="104">
         <f t="shared" ca="1" si="103"/>
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="O32" s="104">
         <f t="shared" ca="1" si="103"/>
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="P32" s="104">
         <f t="shared" ca="1" si="103"/>
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="Q32" s="104">
         <f t="shared" ca="1" si="103"/>
-        <v>23</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -22701,59 +22701,59 @@
       </c>
       <c r="D34" s="105">
         <f ca="1">RANDBETWEEN(20,60)+D33</f>
-        <v>549</v>
+        <v>555</v>
       </c>
       <c r="E34" s="105">
         <f t="shared" ref="E34" ca="1" si="104">RANDBETWEEN(20,60)+E33</f>
-        <v>534</v>
+        <v>520</v>
       </c>
       <c r="F34" s="105">
         <f t="shared" ref="F34" ca="1" si="105">RANDBETWEEN(20,60)+F33</f>
-        <v>529</v>
+        <v>544</v>
       </c>
       <c r="G34" s="105">
         <f t="shared" ref="G34" ca="1" si="106">RANDBETWEEN(20,60)+G33</f>
-        <v>553</v>
+        <v>535</v>
       </c>
       <c r="H34" s="105">
         <f t="shared" ref="H34" ca="1" si="107">RANDBETWEEN(20,60)+H33</f>
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="I34" s="105">
         <f t="shared" ref="I34" ca="1" si="108">RANDBETWEEN(20,60)+I33</f>
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="J34" s="105">
         <f t="shared" ref="J34" ca="1" si="109">RANDBETWEEN(20,60)+J33</f>
-        <v>536</v>
+        <v>523</v>
       </c>
       <c r="K34" s="105">
         <f t="shared" ref="K34" ca="1" si="110">RANDBETWEEN(20,60)+K33</f>
-        <v>542</v>
+        <v>526</v>
       </c>
       <c r="L34" s="105">
         <f t="shared" ref="L34" ca="1" si="111">RANDBETWEEN(20,60)+L33</f>
-        <v>544</v>
+        <v>560</v>
       </c>
       <c r="M34" s="105">
         <f t="shared" ref="M34" ca="1" si="112">RANDBETWEEN(20,60)+M33</f>
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="N34" s="105">
         <f t="shared" ref="N34" ca="1" si="113">RANDBETWEEN(20,60)+N33</f>
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="O34" s="105">
         <f t="shared" ref="O34" ca="1" si="114">RANDBETWEEN(20,60)+O33</f>
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="P34" s="105">
         <f t="shared" ref="P34" ca="1" si="115">RANDBETWEEN(20,60)+P33</f>
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="Q34" s="105">
         <f t="shared" ref="Q34" ca="1" si="116">RANDBETWEEN(20,60)+Q33</f>
-        <v>529</v>
+        <v>531</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
@@ -22768,59 +22768,59 @@
       </c>
       <c r="D35" s="105">
         <f t="shared" ref="D35:Q35" ca="1" si="117">D34-D33</f>
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E35" s="105">
         <f t="shared" ca="1" si="117"/>
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="F35" s="105">
         <f t="shared" ca="1" si="117"/>
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="G35" s="105">
         <f t="shared" ca="1" si="117"/>
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="H35" s="105">
         <f t="shared" ca="1" si="117"/>
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="I35" s="105">
         <f t="shared" ca="1" si="117"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J35" s="105">
         <f t="shared" ca="1" si="117"/>
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="K35" s="105">
         <f t="shared" ca="1" si="117"/>
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="L35" s="105">
         <f t="shared" ca="1" si="117"/>
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="M35" s="105">
         <f t="shared" ca="1" si="117"/>
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="N35" s="105">
         <f t="shared" ca="1" si="117"/>
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="O35" s="105">
         <f t="shared" ca="1" si="117"/>
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="P35" s="105">
         <f t="shared" ca="1" si="117"/>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q35" s="105">
         <f t="shared" ca="1" si="117"/>
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
@@ -22888,23 +22888,23 @@
       </c>
       <c r="D37" s="105">
         <f ca="1">RANDBETWEEN(20,60)+D36</f>
-        <v>526</v>
+        <v>550</v>
       </c>
       <c r="E37" s="105">
         <f t="shared" ref="E37" ca="1" si="118">RANDBETWEEN(20,60)+E36</f>
-        <v>557</v>
+        <v>540</v>
       </c>
       <c r="F37" s="105">
         <f t="shared" ref="F37" ca="1" si="119">RANDBETWEEN(20,60)+F36</f>
-        <v>545</v>
+        <v>550</v>
       </c>
       <c r="G37" s="105">
         <f t="shared" ref="G37" ca="1" si="120">RANDBETWEEN(20,60)+G36</f>
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="H37" s="105">
         <f t="shared" ref="H37" ca="1" si="121">RANDBETWEEN(20,60)+H36</f>
-        <v>545</v>
+        <v>533</v>
       </c>
       <c r="I37" s="105">
         <f t="shared" ref="I37" ca="1" si="122">RANDBETWEEN(20,60)+I36</f>
@@ -22916,31 +22916,31 @@
       </c>
       <c r="K37" s="105">
         <f t="shared" ref="K37" ca="1" si="124">RANDBETWEEN(20,60)+K36</f>
-        <v>535</v>
+        <v>558</v>
       </c>
       <c r="L37" s="105">
         <f t="shared" ref="L37" ca="1" si="125">RANDBETWEEN(20,60)+L36</f>
-        <v>541</v>
+        <v>524</v>
       </c>
       <c r="M37" s="105">
         <f t="shared" ref="M37" ca="1" si="126">RANDBETWEEN(20,60)+M36</f>
-        <v>542</v>
+        <v>532</v>
       </c>
       <c r="N37" s="105">
         <f t="shared" ref="N37" ca="1" si="127">RANDBETWEEN(20,60)+N36</f>
-        <v>551</v>
+        <v>531</v>
       </c>
       <c r="O37" s="105">
         <f t="shared" ref="O37" ca="1" si="128">RANDBETWEEN(20,60)+O36</f>
-        <v>546</v>
+        <v>523</v>
       </c>
       <c r="P37" s="105">
         <f t="shared" ref="P37" ca="1" si="129">RANDBETWEEN(20,60)+P36</f>
-        <v>558</v>
+        <v>527</v>
       </c>
       <c r="Q37" s="105">
         <f t="shared" ref="Q37" ca="1" si="130">RANDBETWEEN(20,60)+Q36</f>
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
@@ -22955,23 +22955,23 @@
       </c>
       <c r="D38" s="105">
         <f t="shared" ref="D38:Q38" ca="1" si="131">D37-D36</f>
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="E38" s="105">
         <f t="shared" ca="1" si="131"/>
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="F38" s="105">
         <f t="shared" ca="1" si="131"/>
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G38" s="105">
         <f t="shared" ca="1" si="131"/>
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H38" s="105">
         <f t="shared" ca="1" si="131"/>
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="I38" s="105">
         <f t="shared" ca="1" si="131"/>
@@ -22983,31 +22983,31 @@
       </c>
       <c r="K38" s="105">
         <f t="shared" ca="1" si="131"/>
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="L38" s="105">
         <f t="shared" ca="1" si="131"/>
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="M38" s="105">
         <f t="shared" ca="1" si="131"/>
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="N38" s="105">
         <f t="shared" ca="1" si="131"/>
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="O38" s="105">
         <f t="shared" ca="1" si="131"/>
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="P38" s="105">
         <f t="shared" ca="1" si="131"/>
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="Q38" s="105">
         <f t="shared" ca="1" si="131"/>
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -23075,59 +23075,59 @@
       </c>
       <c r="D40" s="105">
         <f ca="1">RANDBETWEEN(20,60)+D39</f>
-        <v>542</v>
+        <v>549</v>
       </c>
       <c r="E40" s="105">
         <f t="shared" ref="E40" ca="1" si="132">RANDBETWEEN(20,60)+E39</f>
-        <v>530</v>
+        <v>548</v>
       </c>
       <c r="F40" s="105">
         <f t="shared" ref="F40" ca="1" si="133">RANDBETWEEN(20,60)+F39</f>
-        <v>523</v>
+        <v>549</v>
       </c>
       <c r="G40" s="105">
         <f t="shared" ref="G40" ca="1" si="134">RANDBETWEEN(20,60)+G39</f>
-        <v>555</v>
+        <v>542</v>
       </c>
       <c r="H40" s="105">
         <f t="shared" ref="H40" ca="1" si="135">RANDBETWEEN(20,60)+H39</f>
-        <v>548</v>
+        <v>521</v>
       </c>
       <c r="I40" s="105">
         <f t="shared" ref="I40" ca="1" si="136">RANDBETWEEN(20,60)+I39</f>
-        <v>549</v>
+        <v>525</v>
       </c>
       <c r="J40" s="105">
         <f t="shared" ref="J40" ca="1" si="137">RANDBETWEEN(20,60)+J39</f>
-        <v>548</v>
+        <v>537</v>
       </c>
       <c r="K40" s="105">
         <f t="shared" ref="K40" ca="1" si="138">RANDBETWEEN(20,60)+K39</f>
-        <v>536</v>
+        <v>559</v>
       </c>
       <c r="L40" s="105">
         <f t="shared" ref="L40" ca="1" si="139">RANDBETWEEN(20,60)+L39</f>
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="M40" s="105">
         <f t="shared" ref="M40" ca="1" si="140">RANDBETWEEN(20,60)+M39</f>
-        <v>558</v>
+        <v>545</v>
       </c>
       <c r="N40" s="105">
         <f t="shared" ref="N40" ca="1" si="141">RANDBETWEEN(20,60)+N39</f>
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="O40" s="105">
         <f t="shared" ref="O40" ca="1" si="142">RANDBETWEEN(20,60)+O39</f>
-        <v>525</v>
+        <v>548</v>
       </c>
       <c r="P40" s="105">
         <f t="shared" ref="P40" ca="1" si="143">RANDBETWEEN(20,60)+P39</f>
-        <v>550</v>
+        <v>554</v>
       </c>
       <c r="Q40" s="105">
         <f t="shared" ref="Q40" ca="1" si="144">RANDBETWEEN(20,60)+Q39</f>
-        <v>527</v>
+        <v>545</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
@@ -23142,59 +23142,59 @@
       </c>
       <c r="D41" s="105">
         <f t="shared" ref="D41:Q41" ca="1" si="145">D40-D39</f>
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E41" s="105">
         <f t="shared" ca="1" si="145"/>
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="F41" s="105">
         <f t="shared" ca="1" si="145"/>
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="G41" s="105">
         <f t="shared" ca="1" si="145"/>
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="H41" s="105">
         <f t="shared" ca="1" si="145"/>
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="I41" s="105">
         <f t="shared" ca="1" si="145"/>
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="J41" s="105">
         <f t="shared" ca="1" si="145"/>
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="K41" s="105">
         <f t="shared" ca="1" si="145"/>
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L41" s="105">
         <f t="shared" ca="1" si="145"/>
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="M41" s="105">
         <f t="shared" ca="1" si="145"/>
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="N41" s="105">
         <f t="shared" ca="1" si="145"/>
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O41" s="105">
         <f t="shared" ca="1" si="145"/>
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="P41" s="105">
         <f t="shared" ca="1" si="145"/>
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="Q41" s="105">
         <f t="shared" ca="1" si="145"/>
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
@@ -23262,11 +23262,11 @@
       </c>
       <c r="D43" s="105">
         <f ca="1">RANDBETWEEN(20,60)+D42</f>
-        <v>520</v>
+        <v>553</v>
       </c>
       <c r="E43" s="105">
         <f t="shared" ref="E43" ca="1" si="146">RANDBETWEEN(20,60)+E42</f>
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="F43" s="105">
         <f t="shared" ref="F43" ca="1" si="147">RANDBETWEEN(20,60)+F42</f>
@@ -23274,47 +23274,47 @@
       </c>
       <c r="G43" s="105">
         <f t="shared" ref="G43" ca="1" si="148">RANDBETWEEN(20,60)+G42</f>
-        <v>548</v>
+        <v>522</v>
       </c>
       <c r="H43" s="105">
         <f t="shared" ref="H43" ca="1" si="149">RANDBETWEEN(20,60)+H42</f>
-        <v>530</v>
+        <v>537</v>
       </c>
       <c r="I43" s="105">
         <f t="shared" ref="I43" ca="1" si="150">RANDBETWEEN(20,60)+I42</f>
-        <v>524</v>
+        <v>531</v>
       </c>
       <c r="J43" s="105">
         <f t="shared" ref="J43" ca="1" si="151">RANDBETWEEN(20,60)+J42</f>
-        <v>538</v>
+        <v>550</v>
       </c>
       <c r="K43" s="105">
         <f t="shared" ref="K43" ca="1" si="152">RANDBETWEEN(20,60)+K42</f>
-        <v>524</v>
+        <v>538</v>
       </c>
       <c r="L43" s="105">
         <f t="shared" ref="L43" ca="1" si="153">RANDBETWEEN(20,60)+L42</f>
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="M43" s="105">
         <f t="shared" ref="M43" ca="1" si="154">RANDBETWEEN(20,60)+M42</f>
-        <v>551</v>
+        <v>532</v>
       </c>
       <c r="N43" s="105">
         <f t="shared" ref="N43" ca="1" si="155">RANDBETWEEN(20,60)+N42</f>
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="O43" s="105">
         <f t="shared" ref="O43" ca="1" si="156">RANDBETWEEN(20,60)+O42</f>
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="P43" s="105">
         <f t="shared" ref="P43" ca="1" si="157">RANDBETWEEN(20,60)+P42</f>
-        <v>560</v>
+        <v>543</v>
       </c>
       <c r="Q43" s="105">
         <f t="shared" ref="Q43" ca="1" si="158">RANDBETWEEN(20,60)+Q42</f>
-        <v>547</v>
+        <v>541</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
@@ -23329,11 +23329,11 @@
       </c>
       <c r="D44" s="105">
         <f t="shared" ref="D44:Q44" ca="1" si="159">D43-D42</f>
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="E44" s="105">
         <f t="shared" ca="1" si="159"/>
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F44" s="105">
         <f t="shared" ca="1" si="159"/>
@@ -23341,47 +23341,47 @@
       </c>
       <c r="G44" s="105">
         <f t="shared" ca="1" si="159"/>
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="H44" s="105">
         <f t="shared" ca="1" si="159"/>
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="I44" s="105">
         <f t="shared" ca="1" si="159"/>
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="J44" s="105">
         <f t="shared" ca="1" si="159"/>
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="K44" s="105">
         <f t="shared" ca="1" si="159"/>
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="L44" s="105">
         <f t="shared" ca="1" si="159"/>
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="M44" s="105">
         <f t="shared" ca="1" si="159"/>
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="N44" s="105">
         <f t="shared" ca="1" si="159"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O44" s="105">
         <f t="shared" ca="1" si="159"/>
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="P44" s="105">
         <f t="shared" ca="1" si="159"/>
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="Q44" s="105">
         <f t="shared" ca="1" si="159"/>
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
@@ -23449,55 +23449,55 @@
       </c>
       <c r="D46" s="105">
         <f ca="1">RANDBETWEEN(20,60)+D45</f>
-        <v>558</v>
+        <v>525</v>
       </c>
       <c r="E46" s="105">
         <f t="shared" ref="E46" ca="1" si="160">RANDBETWEEN(20,60)+E45</f>
-        <v>529</v>
+        <v>555</v>
       </c>
       <c r="F46" s="105">
         <f t="shared" ref="F46" ca="1" si="161">RANDBETWEEN(20,60)+F45</f>
-        <v>551</v>
+        <v>530</v>
       </c>
       <c r="G46" s="105">
         <f t="shared" ref="G46" ca="1" si="162">RANDBETWEEN(20,60)+G45</f>
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="H46" s="105">
         <f t="shared" ref="H46" ca="1" si="163">RANDBETWEEN(20,60)+H45</f>
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="I46" s="105">
         <f t="shared" ref="I46" ca="1" si="164">RANDBETWEEN(20,60)+I45</f>
-        <v>542</v>
+        <v>528</v>
       </c>
       <c r="J46" s="105">
         <f t="shared" ref="J46" ca="1" si="165">RANDBETWEEN(20,60)+J45</f>
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="K46" s="105">
         <f t="shared" ref="K46" ca="1" si="166">RANDBETWEEN(20,60)+K45</f>
-        <v>524</v>
+        <v>548</v>
       </c>
       <c r="L46" s="105">
         <f t="shared" ref="L46" ca="1" si="167">RANDBETWEEN(20,60)+L45</f>
-        <v>539</v>
+        <v>528</v>
       </c>
       <c r="M46" s="105">
         <f t="shared" ref="M46" ca="1" si="168">RANDBETWEEN(20,60)+M45</f>
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="N46" s="105">
         <f t="shared" ref="N46" ca="1" si="169">RANDBETWEEN(20,60)+N45</f>
-        <v>527</v>
+        <v>536</v>
       </c>
       <c r="O46" s="105">
         <f t="shared" ref="O46" ca="1" si="170">RANDBETWEEN(20,60)+O45</f>
-        <v>521</v>
+        <v>558</v>
       </c>
       <c r="P46" s="105">
         <f t="shared" ref="P46" ca="1" si="171">RANDBETWEEN(20,60)+P45</f>
-        <v>541</v>
+        <v>557</v>
       </c>
       <c r="Q46" s="105">
         <f t="shared" ref="Q46" ca="1" si="172">RANDBETWEEN(20,60)+Q45</f>
@@ -23516,55 +23516,55 @@
       </c>
       <c r="D47" s="105">
         <f t="shared" ref="D47:Q47" ca="1" si="173">D46-D45</f>
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="E47" s="105">
         <f t="shared" ca="1" si="173"/>
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="F47" s="105">
         <f t="shared" ca="1" si="173"/>
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="G47" s="105">
         <f t="shared" ca="1" si="173"/>
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H47" s="105">
         <f t="shared" ca="1" si="173"/>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I47" s="105">
         <f t="shared" ca="1" si="173"/>
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="J47" s="105">
         <f t="shared" ca="1" si="173"/>
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K47" s="105">
         <f t="shared" ca="1" si="173"/>
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="L47" s="105">
         <f t="shared" ca="1" si="173"/>
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="M47" s="105">
         <f t="shared" ca="1" si="173"/>
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="N47" s="105">
         <f t="shared" ca="1" si="173"/>
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="O47" s="105">
         <f t="shared" ca="1" si="173"/>
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="P47" s="105">
         <f t="shared" ca="1" si="173"/>
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="Q47" s="105">
         <f t="shared" ca="1" si="173"/>

</xml_diff>